<commit_message>
Added functioning links to the responses and more styling to the weidget
</commit_message>
<xml_diff>
--- a/server/src/dataset/OIT Responses.xlsx
+++ b/server/src/dataset/OIT Responses.xlsx
@@ -22,7 +22,8 @@
     <t>Password_reset</t>
   </si>
   <si>
-    <t>Please click on the following link to reset your password. https://myaccount.ucdenver.edu/change-password</t>
+    <t>Please click on the following link to reset your password. 
+&lt;a href="https://myaccount.ucdenver.edu/change-password" target="_blank"&gt;https://myaccount.ucdenver.edu/change-password&lt;/a&gt;</t>
   </si>
   <si>
     <t>Username</t>
@@ -34,7 +35,8 @@
         <color rgb="FF000000"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve">To obtain your username, you can go to the following website and click on 'Forgot my username?' under the 'Next Step button. Your username will be sent to the email you registered your account with. </t>
+      <t xml:space="preserve">To obtain your username, you can go to the following website and click on 'Forgot my username?' under the 'Next Step button. Your username will be sent to the email you registered your account with. 
+</t>
     </r>
     <r>
       <rPr>
@@ -43,20 +45,48 @@
         <sz val="11.0"/>
         <u/>
       </rPr>
-      <t>https://myaccount.ucdenver.edu/change-password</t>
+      <t>&lt;a href="https://myaccount.ucdenver.edu/change-password" target="_blank"&gt;https://myaccount.ucdenver.edu/change-password&lt;/a&gt;</t>
     </r>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Please click on the following link to claim your account. After step 1, you will receive your email address (if your account has already been claimed). https://myaccount.ucdenver.edu/step6.php</t>
+    <t xml:space="preserve">Please click on the following link to claim your account. After step 1, you will receive your email address (If your account has already been claimed). 
+&lt;a href="https://myaccount.ucdenver.edu/step6.php" target="_blank"&gt;https://myaccount.ucdenver.edu/step6.php&lt;/a&gt;
+</t>
   </si>
   <si>
     <t>DUO_Reactivation</t>
   </si>
   <si>
-    <t>To reactivate your DUO account, please click on the following website &gt; scroll down to frequently asked questions &gt; Click on “I upgraded to a new phone and now DUO is not working. How do I reactivate Duo?” and follows these steps https://www.cuanschutz.edu/offices/office-of-information-technology/tools-services/detail-page/multi-factor-authentication--mfa--with-duo. If you continue to have issues, please give us a call at 303-724-4357.</t>
+    <r>
+      <rPr>
+        <rFont val="Arial, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>To reactivate your DUO account, please click on the following website &gt; scroll down to frequently asked questions &gt; Click on “I upgraded to a new phone and now DUO is not working. How do I reactivate Duo?” and follows these steps at: 
+&lt;a href="https://www.cuanschutz.edu/offices/office-of-information-technology/tools-services/multi-factor-authentication--mfa--with-duo" target="_blank"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://www.cuanschutz.edu/offices/office-of-information-technology/tools-services/multi-factor-authentication--mfa--with-duo</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>&lt;/a&gt;
+If you continue to have issues, please give us a call at 303-724-4357.</t>
+    </r>
   </si>
   <si>
     <t>DUO_Change</t>
@@ -80,7 +110,34 @@
     <t>VPN_Access</t>
   </si>
   <si>
-    <t>Please refer to our page on VPN access. https://www.ucdenver.edu/offices/office-of-information-technology/tools-services/remote-access-vpn. If you continue to have issues, please give us a call at 303-724-4357.</t>
+    <r>
+      <rPr>
+        <rFont val="Arial, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Please refer to our page on VPN access. 
+&lt;a href="https://www.cuanschutz.edu/offices/office-of-information-technology/tools-services/detail-page/remote-access-vpn 
+" target="_blank"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial, sans-serif"/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://www.cuanschutz.edu/offices/office-of-information-technology/tools-services/detail-page/remote-access-vpn</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial, sans-serif"/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>&lt;/a&gt;
+If you continue to have issues, please give us a call at 303-724-4357.</t>
+    </r>
   </si>
   <si>
     <t>Locked_account</t>
@@ -137,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -154,6 +211,9 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -407,7 +467,7 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -415,7 +475,7 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -447,7 +507,7 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -468,2976 +528,2978 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="6"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="13">
-      <c r="B13" s="6"/>
+      <c r="B13" s="7"/>
     </row>
     <row r="14">
-      <c r="B14" s="6"/>
+      <c r="B14" s="7"/>
     </row>
     <row r="15">
-      <c r="B15" s="6"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16">
-      <c r="B16" s="6"/>
+      <c r="B16" s="7"/>
     </row>
     <row r="17">
-      <c r="B17" s="6"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18">
-      <c r="B18" s="6"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19">
-      <c r="B19" s="6"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20">
-      <c r="B20" s="6"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21">
-      <c r="B21" s="6"/>
+      <c r="B21" s="7"/>
     </row>
     <row r="22">
-      <c r="B22" s="6"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23">
-      <c r="B23" s="6"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24">
-      <c r="B24" s="6"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25">
-      <c r="B25" s="6"/>
+      <c r="B25" s="7"/>
     </row>
     <row r="26">
-      <c r="B26" s="6"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27">
-      <c r="B27" s="6"/>
+      <c r="B27" s="7"/>
     </row>
     <row r="28">
-      <c r="B28" s="6"/>
+      <c r="B28" s="7"/>
     </row>
     <row r="29">
-      <c r="B29" s="6"/>
+      <c r="B29" s="7"/>
     </row>
     <row r="30">
-      <c r="B30" s="6"/>
+      <c r="B30" s="7"/>
     </row>
     <row r="31">
-      <c r="B31" s="6"/>
+      <c r="B31" s="7"/>
     </row>
     <row r="32">
-      <c r="B32" s="6"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33">
-      <c r="B33" s="6"/>
+      <c r="B33" s="7"/>
     </row>
     <row r="34">
-      <c r="B34" s="6"/>
+      <c r="B34" s="7"/>
     </row>
     <row r="35">
-      <c r="B35" s="6"/>
+      <c r="B35" s="7"/>
     </row>
     <row r="36">
-      <c r="B36" s="6"/>
+      <c r="B36" s="7"/>
     </row>
     <row r="37">
-      <c r="B37" s="6"/>
+      <c r="B37" s="7"/>
     </row>
     <row r="38">
-      <c r="B38" s="6"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39">
-      <c r="B39" s="6"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40">
-      <c r="B40" s="6"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41">
-      <c r="B41" s="6"/>
+      <c r="B41" s="7"/>
     </row>
     <row r="42">
-      <c r="B42" s="6"/>
+      <c r="B42" s="7"/>
     </row>
     <row r="43">
-      <c r="B43" s="6"/>
+      <c r="B43" s="7"/>
     </row>
     <row r="44">
-      <c r="B44" s="6"/>
+      <c r="B44" s="7"/>
     </row>
     <row r="45">
-      <c r="B45" s="6"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="46">
-      <c r="B46" s="6"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47">
-      <c r="B47" s="6"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48">
-      <c r="B48" s="6"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49">
-      <c r="B49" s="6"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50">
-      <c r="B50" s="6"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51">
-      <c r="B51" s="6"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52">
-      <c r="B52" s="6"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53">
-      <c r="B53" s="6"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54">
-      <c r="B54" s="6"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55">
-      <c r="B55" s="6"/>
+      <c r="B55" s="7"/>
     </row>
     <row r="56">
-      <c r="B56" s="6"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="57">
-      <c r="B57" s="6"/>
+      <c r="B57" s="7"/>
     </row>
     <row r="58">
-      <c r="B58" s="6"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59">
-      <c r="B59" s="6"/>
+      <c r="B59" s="7"/>
     </row>
     <row r="60">
-      <c r="B60" s="6"/>
+      <c r="B60" s="7"/>
     </row>
     <row r="61">
-      <c r="B61" s="6"/>
+      <c r="B61" s="7"/>
     </row>
     <row r="62">
-      <c r="B62" s="6"/>
+      <c r="B62" s="7"/>
     </row>
     <row r="63">
-      <c r="B63" s="6"/>
+      <c r="B63" s="7"/>
     </row>
     <row r="64">
-      <c r="B64" s="6"/>
+      <c r="B64" s="7"/>
     </row>
     <row r="65">
-      <c r="B65" s="6"/>
+      <c r="B65" s="7"/>
     </row>
     <row r="66">
-      <c r="B66" s="6"/>
+      <c r="B66" s="7"/>
     </row>
     <row r="67">
-      <c r="B67" s="6"/>
+      <c r="B67" s="7"/>
     </row>
     <row r="68">
-      <c r="B68" s="6"/>
+      <c r="B68" s="7"/>
     </row>
     <row r="69">
-      <c r="B69" s="6"/>
+      <c r="B69" s="7"/>
     </row>
     <row r="70">
-      <c r="B70" s="6"/>
+      <c r="B70" s="7"/>
     </row>
     <row r="71">
-      <c r="B71" s="6"/>
+      <c r="B71" s="7"/>
     </row>
     <row r="72">
-      <c r="B72" s="6"/>
+      <c r="B72" s="7"/>
     </row>
     <row r="73">
-      <c r="B73" s="6"/>
+      <c r="B73" s="7"/>
     </row>
     <row r="74">
-      <c r="B74" s="6"/>
+      <c r="B74" s="7"/>
     </row>
     <row r="75">
-      <c r="B75" s="6"/>
+      <c r="B75" s="7"/>
     </row>
     <row r="76">
-      <c r="B76" s="6"/>
+      <c r="B76" s="7"/>
     </row>
     <row r="77">
-      <c r="B77" s="6"/>
+      <c r="B77" s="7"/>
     </row>
     <row r="78">
-      <c r="B78" s="6"/>
+      <c r="B78" s="7"/>
     </row>
     <row r="79">
-      <c r="B79" s="6"/>
+      <c r="B79" s="7"/>
     </row>
     <row r="80">
-      <c r="B80" s="6"/>
+      <c r="B80" s="7"/>
     </row>
     <row r="81">
-      <c r="B81" s="6"/>
+      <c r="B81" s="7"/>
     </row>
     <row r="82">
-      <c r="B82" s="6"/>
+      <c r="B82" s="7"/>
     </row>
     <row r="83">
-      <c r="B83" s="6"/>
+      <c r="B83" s="7"/>
     </row>
     <row r="84">
-      <c r="B84" s="6"/>
+      <c r="B84" s="7"/>
     </row>
     <row r="85">
-      <c r="B85" s="6"/>
+      <c r="B85" s="7"/>
     </row>
     <row r="86">
-      <c r="B86" s="6"/>
+      <c r="B86" s="7"/>
     </row>
     <row r="87">
-      <c r="B87" s="6"/>
+      <c r="B87" s="7"/>
     </row>
     <row r="88">
-      <c r="B88" s="6"/>
+      <c r="B88" s="7"/>
     </row>
     <row r="89">
-      <c r="B89" s="6"/>
+      <c r="B89" s="7"/>
     </row>
     <row r="90">
-      <c r="B90" s="6"/>
+      <c r="B90" s="7"/>
     </row>
     <row r="91">
-      <c r="B91" s="6"/>
+      <c r="B91" s="7"/>
     </row>
     <row r="92">
-      <c r="B92" s="6"/>
+      <c r="B92" s="7"/>
     </row>
     <row r="93">
-      <c r="B93" s="6"/>
+      <c r="B93" s="7"/>
     </row>
     <row r="94">
-      <c r="B94" s="6"/>
+      <c r="B94" s="7"/>
     </row>
     <row r="95">
-      <c r="B95" s="6"/>
+      <c r="B95" s="7"/>
     </row>
     <row r="96">
-      <c r="B96" s="6"/>
+      <c r="B96" s="7"/>
     </row>
     <row r="97">
-      <c r="B97" s="6"/>
+      <c r="B97" s="7"/>
     </row>
     <row r="98">
-      <c r="B98" s="6"/>
+      <c r="B98" s="7"/>
     </row>
     <row r="99">
-      <c r="B99" s="6"/>
+      <c r="B99" s="7"/>
     </row>
     <row r="100">
-      <c r="B100" s="6"/>
+      <c r="B100" s="7"/>
     </row>
     <row r="101">
-      <c r="B101" s="6"/>
+      <c r="B101" s="7"/>
     </row>
     <row r="102">
-      <c r="B102" s="6"/>
+      <c r="B102" s="7"/>
     </row>
     <row r="103">
-      <c r="B103" s="6"/>
+      <c r="B103" s="7"/>
     </row>
     <row r="104">
-      <c r="B104" s="6"/>
+      <c r="B104" s="7"/>
     </row>
     <row r="105">
-      <c r="B105" s="6"/>
+      <c r="B105" s="7"/>
     </row>
     <row r="106">
-      <c r="B106" s="6"/>
+      <c r="B106" s="7"/>
     </row>
     <row r="107">
-      <c r="B107" s="6"/>
+      <c r="B107" s="7"/>
     </row>
     <row r="108">
-      <c r="B108" s="6"/>
+      <c r="B108" s="7"/>
     </row>
     <row r="109">
-      <c r="B109" s="6"/>
+      <c r="B109" s="7"/>
     </row>
     <row r="110">
-      <c r="B110" s="6"/>
+      <c r="B110" s="7"/>
     </row>
     <row r="111">
-      <c r="B111" s="6"/>
+      <c r="B111" s="7"/>
     </row>
     <row r="112">
-      <c r="B112" s="6"/>
+      <c r="B112" s="7"/>
     </row>
     <row r="113">
-      <c r="B113" s="6"/>
+      <c r="B113" s="7"/>
     </row>
     <row r="114">
-      <c r="B114" s="6"/>
+      <c r="B114" s="7"/>
     </row>
     <row r="115">
-      <c r="B115" s="6"/>
+      <c r="B115" s="7"/>
     </row>
     <row r="116">
-      <c r="B116" s="6"/>
+      <c r="B116" s="7"/>
     </row>
     <row r="117">
-      <c r="B117" s="6"/>
+      <c r="B117" s="7"/>
     </row>
     <row r="118">
-      <c r="B118" s="6"/>
+      <c r="B118" s="7"/>
     </row>
     <row r="119">
-      <c r="B119" s="6"/>
+      <c r="B119" s="7"/>
     </row>
     <row r="120">
-      <c r="B120" s="6"/>
+      <c r="B120" s="7"/>
     </row>
     <row r="121">
-      <c r="B121" s="6"/>
+      <c r="B121" s="7"/>
     </row>
     <row r="122">
-      <c r="B122" s="6"/>
+      <c r="B122" s="7"/>
     </row>
     <row r="123">
-      <c r="B123" s="6"/>
+      <c r="B123" s="7"/>
     </row>
     <row r="124">
-      <c r="B124" s="6"/>
+      <c r="B124" s="7"/>
     </row>
     <row r="125">
-      <c r="B125" s="6"/>
+      <c r="B125" s="7"/>
     </row>
     <row r="126">
-      <c r="B126" s="6"/>
+      <c r="B126" s="7"/>
     </row>
     <row r="127">
-      <c r="B127" s="6"/>
+      <c r="B127" s="7"/>
     </row>
     <row r="128">
-      <c r="B128" s="6"/>
+      <c r="B128" s="7"/>
     </row>
     <row r="129">
-      <c r="B129" s="6"/>
+      <c r="B129" s="7"/>
     </row>
     <row r="130">
-      <c r="B130" s="6"/>
+      <c r="B130" s="7"/>
     </row>
     <row r="131">
-      <c r="B131" s="6"/>
+      <c r="B131" s="7"/>
     </row>
     <row r="132">
-      <c r="B132" s="6"/>
+      <c r="B132" s="7"/>
     </row>
     <row r="133">
-      <c r="B133" s="6"/>
+      <c r="B133" s="7"/>
     </row>
     <row r="134">
-      <c r="B134" s="6"/>
+      <c r="B134" s="7"/>
     </row>
     <row r="135">
-      <c r="B135" s="6"/>
+      <c r="B135" s="7"/>
     </row>
     <row r="136">
-      <c r="B136" s="6"/>
+      <c r="B136" s="7"/>
     </row>
     <row r="137">
-      <c r="B137" s="6"/>
+      <c r="B137" s="7"/>
     </row>
     <row r="138">
-      <c r="B138" s="6"/>
+      <c r="B138" s="7"/>
     </row>
     <row r="139">
-      <c r="B139" s="6"/>
+      <c r="B139" s="7"/>
     </row>
     <row r="140">
-      <c r="B140" s="6"/>
+      <c r="B140" s="7"/>
     </row>
     <row r="141">
-      <c r="B141" s="6"/>
+      <c r="B141" s="7"/>
     </row>
     <row r="142">
-      <c r="B142" s="6"/>
+      <c r="B142" s="7"/>
     </row>
     <row r="143">
-      <c r="B143" s="6"/>
+      <c r="B143" s="7"/>
     </row>
     <row r="144">
-      <c r="B144" s="6"/>
+      <c r="B144" s="7"/>
     </row>
     <row r="145">
-      <c r="B145" s="6"/>
+      <c r="B145" s="7"/>
     </row>
     <row r="146">
-      <c r="B146" s="6"/>
+      <c r="B146" s="7"/>
     </row>
     <row r="147">
-      <c r="B147" s="6"/>
+      <c r="B147" s="7"/>
     </row>
     <row r="148">
-      <c r="B148" s="6"/>
+      <c r="B148" s="7"/>
     </row>
     <row r="149">
-      <c r="B149" s="6"/>
+      <c r="B149" s="7"/>
     </row>
     <row r="150">
-      <c r="B150" s="6"/>
+      <c r="B150" s="7"/>
     </row>
     <row r="151">
-      <c r="B151" s="6"/>
+      <c r="B151" s="7"/>
     </row>
     <row r="152">
-      <c r="B152" s="6"/>
+      <c r="B152" s="7"/>
     </row>
     <row r="153">
-      <c r="B153" s="6"/>
+      <c r="B153" s="7"/>
     </row>
     <row r="154">
-      <c r="B154" s="6"/>
+      <c r="B154" s="7"/>
     </row>
     <row r="155">
-      <c r="B155" s="6"/>
+      <c r="B155" s="7"/>
     </row>
     <row r="156">
-      <c r="B156" s="6"/>
+      <c r="B156" s="7"/>
     </row>
     <row r="157">
-      <c r="B157" s="6"/>
+      <c r="B157" s="7"/>
     </row>
     <row r="158">
-      <c r="B158" s="6"/>
+      <c r="B158" s="7"/>
     </row>
     <row r="159">
-      <c r="B159" s="6"/>
+      <c r="B159" s="7"/>
     </row>
     <row r="160">
-      <c r="B160" s="6"/>
+      <c r="B160" s="7"/>
     </row>
     <row r="161">
-      <c r="B161" s="6"/>
+      <c r="B161" s="7"/>
     </row>
     <row r="162">
-      <c r="B162" s="6"/>
+      <c r="B162" s="7"/>
     </row>
     <row r="163">
-      <c r="B163" s="6"/>
+      <c r="B163" s="7"/>
     </row>
     <row r="164">
-      <c r="B164" s="6"/>
+      <c r="B164" s="7"/>
     </row>
     <row r="165">
-      <c r="B165" s="6"/>
+      <c r="B165" s="7"/>
     </row>
     <row r="166">
-      <c r="B166" s="6"/>
+      <c r="B166" s="7"/>
     </row>
     <row r="167">
-      <c r="B167" s="6"/>
+      <c r="B167" s="7"/>
     </row>
     <row r="168">
-      <c r="B168" s="6"/>
+      <c r="B168" s="7"/>
     </row>
     <row r="169">
-      <c r="B169" s="6"/>
+      <c r="B169" s="7"/>
     </row>
     <row r="170">
-      <c r="B170" s="6"/>
+      <c r="B170" s="7"/>
     </row>
     <row r="171">
-      <c r="B171" s="6"/>
+      <c r="B171" s="7"/>
     </row>
     <row r="172">
-      <c r="B172" s="6"/>
+      <c r="B172" s="7"/>
     </row>
     <row r="173">
-      <c r="B173" s="6"/>
+      <c r="B173" s="7"/>
     </row>
     <row r="174">
-      <c r="B174" s="6"/>
+      <c r="B174" s="7"/>
     </row>
     <row r="175">
-      <c r="B175" s="6"/>
+      <c r="B175" s="7"/>
     </row>
     <row r="176">
-      <c r="B176" s="6"/>
+      <c r="B176" s="7"/>
     </row>
     <row r="177">
-      <c r="B177" s="6"/>
+      <c r="B177" s="7"/>
     </row>
     <row r="178">
-      <c r="B178" s="6"/>
+      <c r="B178" s="7"/>
     </row>
     <row r="179">
-      <c r="B179" s="6"/>
+      <c r="B179" s="7"/>
     </row>
     <row r="180">
-      <c r="B180" s="6"/>
+      <c r="B180" s="7"/>
     </row>
     <row r="181">
-      <c r="B181" s="6"/>
+      <c r="B181" s="7"/>
     </row>
     <row r="182">
-      <c r="B182" s="6"/>
+      <c r="B182" s="7"/>
     </row>
     <row r="183">
-      <c r="B183" s="6"/>
+      <c r="B183" s="7"/>
     </row>
     <row r="184">
-      <c r="B184" s="6"/>
+      <c r="B184" s="7"/>
     </row>
     <row r="185">
-      <c r="B185" s="6"/>
+      <c r="B185" s="7"/>
     </row>
     <row r="186">
-      <c r="B186" s="6"/>
+      <c r="B186" s="7"/>
     </row>
     <row r="187">
-      <c r="B187" s="6"/>
+      <c r="B187" s="7"/>
     </row>
     <row r="188">
-      <c r="B188" s="6"/>
+      <c r="B188" s="7"/>
     </row>
     <row r="189">
-      <c r="B189" s="6"/>
+      <c r="B189" s="7"/>
     </row>
     <row r="190">
-      <c r="B190" s="6"/>
+      <c r="B190" s="7"/>
     </row>
     <row r="191">
-      <c r="B191" s="6"/>
+      <c r="B191" s="7"/>
     </row>
     <row r="192">
-      <c r="B192" s="6"/>
+      <c r="B192" s="7"/>
     </row>
     <row r="193">
-      <c r="B193" s="6"/>
+      <c r="B193" s="7"/>
     </row>
     <row r="194">
-      <c r="B194" s="6"/>
+      <c r="B194" s="7"/>
     </row>
     <row r="195">
-      <c r="B195" s="6"/>
+      <c r="B195" s="7"/>
     </row>
     <row r="196">
-      <c r="B196" s="6"/>
+      <c r="B196" s="7"/>
     </row>
     <row r="197">
-      <c r="B197" s="6"/>
+      <c r="B197" s="7"/>
     </row>
     <row r="198">
-      <c r="B198" s="6"/>
+      <c r="B198" s="7"/>
     </row>
     <row r="199">
-      <c r="B199" s="6"/>
+      <c r="B199" s="7"/>
     </row>
     <row r="200">
-      <c r="B200" s="6"/>
+      <c r="B200" s="7"/>
     </row>
     <row r="201">
-      <c r="B201" s="6"/>
+      <c r="B201" s="7"/>
     </row>
     <row r="202">
-      <c r="B202" s="6"/>
+      <c r="B202" s="7"/>
     </row>
     <row r="203">
-      <c r="B203" s="6"/>
+      <c r="B203" s="7"/>
     </row>
     <row r="204">
-      <c r="B204" s="6"/>
+      <c r="B204" s="7"/>
     </row>
     <row r="205">
-      <c r="B205" s="6"/>
+      <c r="B205" s="7"/>
     </row>
     <row r="206">
-      <c r="B206" s="6"/>
+      <c r="B206" s="7"/>
     </row>
     <row r="207">
-      <c r="B207" s="6"/>
+      <c r="B207" s="7"/>
     </row>
     <row r="208">
-      <c r="B208" s="6"/>
+      <c r="B208" s="7"/>
     </row>
     <row r="209">
-      <c r="B209" s="6"/>
+      <c r="B209" s="7"/>
     </row>
     <row r="210">
-      <c r="B210" s="6"/>
+      <c r="B210" s="7"/>
     </row>
     <row r="211">
-      <c r="B211" s="6"/>
+      <c r="B211" s="7"/>
     </row>
     <row r="212">
-      <c r="B212" s="6"/>
+      <c r="B212" s="7"/>
     </row>
     <row r="213">
-      <c r="B213" s="6"/>
+      <c r="B213" s="7"/>
     </row>
     <row r="214">
-      <c r="B214" s="6"/>
+      <c r="B214" s="7"/>
     </row>
     <row r="215">
-      <c r="B215" s="6"/>
+      <c r="B215" s="7"/>
     </row>
     <row r="216">
-      <c r="B216" s="6"/>
+      <c r="B216" s="7"/>
     </row>
     <row r="217">
-      <c r="B217" s="6"/>
+      <c r="B217" s="7"/>
     </row>
     <row r="218">
-      <c r="B218" s="6"/>
+      <c r="B218" s="7"/>
     </row>
     <row r="219">
-      <c r="B219" s="6"/>
+      <c r="B219" s="7"/>
     </row>
     <row r="220">
-      <c r="B220" s="6"/>
+      <c r="B220" s="7"/>
     </row>
     <row r="221">
-      <c r="B221" s="6"/>
+      <c r="B221" s="7"/>
     </row>
     <row r="222">
-      <c r="B222" s="6"/>
+      <c r="B222" s="7"/>
     </row>
     <row r="223">
-      <c r="B223" s="6"/>
+      <c r="B223" s="7"/>
     </row>
     <row r="224">
-      <c r="B224" s="6"/>
+      <c r="B224" s="7"/>
     </row>
     <row r="225">
-      <c r="B225" s="6"/>
+      <c r="B225" s="7"/>
     </row>
     <row r="226">
-      <c r="B226" s="6"/>
+      <c r="B226" s="7"/>
     </row>
     <row r="227">
-      <c r="B227" s="6"/>
+      <c r="B227" s="7"/>
     </row>
     <row r="228">
-      <c r="B228" s="6"/>
+      <c r="B228" s="7"/>
     </row>
     <row r="229">
-      <c r="B229" s="6"/>
+      <c r="B229" s="7"/>
     </row>
     <row r="230">
-      <c r="B230" s="6"/>
+      <c r="B230" s="7"/>
     </row>
     <row r="231">
-      <c r="B231" s="6"/>
+      <c r="B231" s="7"/>
     </row>
     <row r="232">
-      <c r="B232" s="6"/>
+      <c r="B232" s="7"/>
     </row>
     <row r="233">
-      <c r="B233" s="6"/>
+      <c r="B233" s="7"/>
     </row>
     <row r="234">
-      <c r="B234" s="6"/>
+      <c r="B234" s="7"/>
     </row>
     <row r="235">
-      <c r="B235" s="6"/>
+      <c r="B235" s="7"/>
     </row>
     <row r="236">
-      <c r="B236" s="6"/>
+      <c r="B236" s="7"/>
     </row>
     <row r="237">
-      <c r="B237" s="6"/>
+      <c r="B237" s="7"/>
     </row>
     <row r="238">
-      <c r="B238" s="6"/>
+      <c r="B238" s="7"/>
     </row>
     <row r="239">
-      <c r="B239" s="6"/>
+      <c r="B239" s="7"/>
     </row>
     <row r="240">
-      <c r="B240" s="6"/>
+      <c r="B240" s="7"/>
     </row>
     <row r="241">
-      <c r="B241" s="6"/>
+      <c r="B241" s="7"/>
     </row>
     <row r="242">
-      <c r="B242" s="6"/>
+      <c r="B242" s="7"/>
     </row>
     <row r="243">
-      <c r="B243" s="6"/>
+      <c r="B243" s="7"/>
     </row>
     <row r="244">
-      <c r="B244" s="6"/>
+      <c r="B244" s="7"/>
     </row>
     <row r="245">
-      <c r="B245" s="6"/>
+      <c r="B245" s="7"/>
     </row>
     <row r="246">
-      <c r="B246" s="6"/>
+      <c r="B246" s="7"/>
     </row>
     <row r="247">
-      <c r="B247" s="6"/>
+      <c r="B247" s="7"/>
     </row>
     <row r="248">
-      <c r="B248" s="6"/>
+      <c r="B248" s="7"/>
     </row>
     <row r="249">
-      <c r="B249" s="6"/>
+      <c r="B249" s="7"/>
     </row>
     <row r="250">
-      <c r="B250" s="6"/>
+      <c r="B250" s="7"/>
     </row>
     <row r="251">
-      <c r="B251" s="6"/>
+      <c r="B251" s="7"/>
     </row>
     <row r="252">
-      <c r="B252" s="6"/>
+      <c r="B252" s="7"/>
     </row>
     <row r="253">
-      <c r="B253" s="6"/>
+      <c r="B253" s="7"/>
     </row>
     <row r="254">
-      <c r="B254" s="6"/>
+      <c r="B254" s="7"/>
     </row>
     <row r="255">
-      <c r="B255" s="6"/>
+      <c r="B255" s="7"/>
     </row>
     <row r="256">
-      <c r="B256" s="6"/>
+      <c r="B256" s="7"/>
     </row>
     <row r="257">
-      <c r="B257" s="6"/>
+      <c r="B257" s="7"/>
     </row>
     <row r="258">
-      <c r="B258" s="6"/>
+      <c r="B258" s="7"/>
     </row>
     <row r="259">
-      <c r="B259" s="6"/>
+      <c r="B259" s="7"/>
     </row>
     <row r="260">
-      <c r="B260" s="6"/>
+      <c r="B260" s="7"/>
     </row>
     <row r="261">
-      <c r="B261" s="6"/>
+      <c r="B261" s="7"/>
     </row>
     <row r="262">
-      <c r="B262" s="6"/>
+      <c r="B262" s="7"/>
     </row>
     <row r="263">
-      <c r="B263" s="6"/>
+      <c r="B263" s="7"/>
     </row>
     <row r="264">
-      <c r="B264" s="6"/>
+      <c r="B264" s="7"/>
     </row>
     <row r="265">
-      <c r="B265" s="6"/>
+      <c r="B265" s="7"/>
     </row>
     <row r="266">
-      <c r="B266" s="6"/>
+      <c r="B266" s="7"/>
     </row>
     <row r="267">
-      <c r="B267" s="6"/>
+      <c r="B267" s="7"/>
     </row>
     <row r="268">
-      <c r="B268" s="6"/>
+      <c r="B268" s="7"/>
     </row>
     <row r="269">
-      <c r="B269" s="6"/>
+      <c r="B269" s="7"/>
     </row>
     <row r="270">
-      <c r="B270" s="6"/>
+      <c r="B270" s="7"/>
     </row>
     <row r="271">
-      <c r="B271" s="6"/>
+      <c r="B271" s="7"/>
     </row>
     <row r="272">
-      <c r="B272" s="6"/>
+      <c r="B272" s="7"/>
     </row>
     <row r="273">
-      <c r="B273" s="6"/>
+      <c r="B273" s="7"/>
     </row>
     <row r="274">
-      <c r="B274" s="6"/>
+      <c r="B274" s="7"/>
     </row>
     <row r="275">
-      <c r="B275" s="6"/>
+      <c r="B275" s="7"/>
     </row>
     <row r="276">
-      <c r="B276" s="6"/>
+      <c r="B276" s="7"/>
     </row>
     <row r="277">
-      <c r="B277" s="6"/>
+      <c r="B277" s="7"/>
     </row>
     <row r="278">
-      <c r="B278" s="6"/>
+      <c r="B278" s="7"/>
     </row>
     <row r="279">
-      <c r="B279" s="6"/>
+      <c r="B279" s="7"/>
     </row>
     <row r="280">
-      <c r="B280" s="6"/>
+      <c r="B280" s="7"/>
     </row>
     <row r="281">
-      <c r="B281" s="6"/>
+      <c r="B281" s="7"/>
     </row>
     <row r="282">
-      <c r="B282" s="6"/>
+      <c r="B282" s="7"/>
     </row>
     <row r="283">
-      <c r="B283" s="6"/>
+      <c r="B283" s="7"/>
     </row>
     <row r="284">
-      <c r="B284" s="6"/>
+      <c r="B284" s="7"/>
     </row>
     <row r="285">
-      <c r="B285" s="6"/>
+      <c r="B285" s="7"/>
     </row>
     <row r="286">
-      <c r="B286" s="6"/>
+      <c r="B286" s="7"/>
     </row>
     <row r="287">
-      <c r="B287" s="6"/>
+      <c r="B287" s="7"/>
     </row>
     <row r="288">
-      <c r="B288" s="6"/>
+      <c r="B288" s="7"/>
     </row>
     <row r="289">
-      <c r="B289" s="6"/>
+      <c r="B289" s="7"/>
     </row>
     <row r="290">
-      <c r="B290" s="6"/>
+      <c r="B290" s="7"/>
     </row>
     <row r="291">
-      <c r="B291" s="6"/>
+      <c r="B291" s="7"/>
     </row>
     <row r="292">
-      <c r="B292" s="6"/>
+      <c r="B292" s="7"/>
     </row>
     <row r="293">
-      <c r="B293" s="6"/>
+      <c r="B293" s="7"/>
     </row>
     <row r="294">
-      <c r="B294" s="6"/>
+      <c r="B294" s="7"/>
     </row>
     <row r="295">
-      <c r="B295" s="6"/>
+      <c r="B295" s="7"/>
     </row>
     <row r="296">
-      <c r="B296" s="6"/>
+      <c r="B296" s="7"/>
     </row>
     <row r="297">
-      <c r="B297" s="6"/>
+      <c r="B297" s="7"/>
     </row>
     <row r="298">
-      <c r="B298" s="6"/>
+      <c r="B298" s="7"/>
     </row>
     <row r="299">
-      <c r="B299" s="6"/>
+      <c r="B299" s="7"/>
     </row>
     <row r="300">
-      <c r="B300" s="6"/>
+      <c r="B300" s="7"/>
     </row>
     <row r="301">
-      <c r="B301" s="6"/>
+      <c r="B301" s="7"/>
     </row>
     <row r="302">
-      <c r="B302" s="6"/>
+      <c r="B302" s="7"/>
     </row>
     <row r="303">
-      <c r="B303" s="6"/>
+      <c r="B303" s="7"/>
     </row>
     <row r="304">
-      <c r="B304" s="6"/>
+      <c r="B304" s="7"/>
     </row>
     <row r="305">
-      <c r="B305" s="6"/>
+      <c r="B305" s="7"/>
     </row>
     <row r="306">
-      <c r="B306" s="6"/>
+      <c r="B306" s="7"/>
     </row>
     <row r="307">
-      <c r="B307" s="6"/>
+      <c r="B307" s="7"/>
     </row>
     <row r="308">
-      <c r="B308" s="6"/>
+      <c r="B308" s="7"/>
     </row>
     <row r="309">
-      <c r="B309" s="6"/>
+      <c r="B309" s="7"/>
     </row>
     <row r="310">
-      <c r="B310" s="6"/>
+      <c r="B310" s="7"/>
     </row>
     <row r="311">
-      <c r="B311" s="6"/>
+      <c r="B311" s="7"/>
     </row>
     <row r="312">
-      <c r="B312" s="6"/>
+      <c r="B312" s="7"/>
     </row>
     <row r="313">
-      <c r="B313" s="6"/>
+      <c r="B313" s="7"/>
     </row>
     <row r="314">
-      <c r="B314" s="6"/>
+      <c r="B314" s="7"/>
     </row>
     <row r="315">
-      <c r="B315" s="6"/>
+      <c r="B315" s="7"/>
     </row>
     <row r="316">
-      <c r="B316" s="6"/>
+      <c r="B316" s="7"/>
     </row>
     <row r="317">
-      <c r="B317" s="6"/>
+      <c r="B317" s="7"/>
     </row>
     <row r="318">
-      <c r="B318" s="6"/>
+      <c r="B318" s="7"/>
     </row>
     <row r="319">
-      <c r="B319" s="6"/>
+      <c r="B319" s="7"/>
     </row>
     <row r="320">
-      <c r="B320" s="6"/>
+      <c r="B320" s="7"/>
     </row>
     <row r="321">
-      <c r="B321" s="6"/>
+      <c r="B321" s="7"/>
     </row>
     <row r="322">
-      <c r="B322" s="6"/>
+      <c r="B322" s="7"/>
     </row>
     <row r="323">
-      <c r="B323" s="6"/>
+      <c r="B323" s="7"/>
     </row>
     <row r="324">
-      <c r="B324" s="6"/>
+      <c r="B324" s="7"/>
     </row>
     <row r="325">
-      <c r="B325" s="6"/>
+      <c r="B325" s="7"/>
     </row>
     <row r="326">
-      <c r="B326" s="6"/>
+      <c r="B326" s="7"/>
     </row>
     <row r="327">
-      <c r="B327" s="6"/>
+      <c r="B327" s="7"/>
     </row>
     <row r="328">
-      <c r="B328" s="6"/>
+      <c r="B328" s="7"/>
     </row>
     <row r="329">
-      <c r="B329" s="6"/>
+      <c r="B329" s="7"/>
     </row>
     <row r="330">
-      <c r="B330" s="6"/>
+      <c r="B330" s="7"/>
     </row>
     <row r="331">
-      <c r="B331" s="6"/>
+      <c r="B331" s="7"/>
     </row>
     <row r="332">
-      <c r="B332" s="6"/>
+      <c r="B332" s="7"/>
     </row>
     <row r="333">
-      <c r="B333" s="6"/>
+      <c r="B333" s="7"/>
     </row>
     <row r="334">
-      <c r="B334" s="6"/>
+      <c r="B334" s="7"/>
     </row>
     <row r="335">
-      <c r="B335" s="6"/>
+      <c r="B335" s="7"/>
     </row>
     <row r="336">
-      <c r="B336" s="6"/>
+      <c r="B336" s="7"/>
     </row>
     <row r="337">
-      <c r="B337" s="6"/>
+      <c r="B337" s="7"/>
     </row>
     <row r="338">
-      <c r="B338" s="6"/>
+      <c r="B338" s="7"/>
     </row>
     <row r="339">
-      <c r="B339" s="6"/>
+      <c r="B339" s="7"/>
     </row>
     <row r="340">
-      <c r="B340" s="6"/>
+      <c r="B340" s="7"/>
     </row>
     <row r="341">
-      <c r="B341" s="6"/>
+      <c r="B341" s="7"/>
     </row>
     <row r="342">
-      <c r="B342" s="6"/>
+      <c r="B342" s="7"/>
     </row>
     <row r="343">
-      <c r="B343" s="6"/>
+      <c r="B343" s="7"/>
     </row>
     <row r="344">
-      <c r="B344" s="6"/>
+      <c r="B344" s="7"/>
     </row>
     <row r="345">
-      <c r="B345" s="6"/>
+      <c r="B345" s="7"/>
     </row>
     <row r="346">
-      <c r="B346" s="6"/>
+      <c r="B346" s="7"/>
     </row>
     <row r="347">
-      <c r="B347" s="6"/>
+      <c r="B347" s="7"/>
     </row>
     <row r="348">
-      <c r="B348" s="6"/>
+      <c r="B348" s="7"/>
     </row>
     <row r="349">
-      <c r="B349" s="6"/>
+      <c r="B349" s="7"/>
     </row>
     <row r="350">
-      <c r="B350" s="6"/>
+      <c r="B350" s="7"/>
     </row>
     <row r="351">
-      <c r="B351" s="6"/>
+      <c r="B351" s="7"/>
     </row>
     <row r="352">
-      <c r="B352" s="6"/>
+      <c r="B352" s="7"/>
     </row>
     <row r="353">
-      <c r="B353" s="6"/>
+      <c r="B353" s="7"/>
     </row>
     <row r="354">
-      <c r="B354" s="6"/>
+      <c r="B354" s="7"/>
     </row>
     <row r="355">
-      <c r="B355" s="6"/>
+      <c r="B355" s="7"/>
     </row>
     <row r="356">
-      <c r="B356" s="6"/>
+      <c r="B356" s="7"/>
     </row>
     <row r="357">
-      <c r="B357" s="6"/>
+      <c r="B357" s="7"/>
     </row>
     <row r="358">
-      <c r="B358" s="6"/>
+      <c r="B358" s="7"/>
     </row>
     <row r="359">
-      <c r="B359" s="6"/>
+      <c r="B359" s="7"/>
     </row>
     <row r="360">
-      <c r="B360" s="6"/>
+      <c r="B360" s="7"/>
     </row>
     <row r="361">
-      <c r="B361" s="6"/>
+      <c r="B361" s="7"/>
     </row>
     <row r="362">
-      <c r="B362" s="6"/>
+      <c r="B362" s="7"/>
     </row>
     <row r="363">
-      <c r="B363" s="6"/>
+      <c r="B363" s="7"/>
     </row>
     <row r="364">
-      <c r="B364" s="6"/>
+      <c r="B364" s="7"/>
     </row>
     <row r="365">
-      <c r="B365" s="6"/>
+      <c r="B365" s="7"/>
     </row>
     <row r="366">
-      <c r="B366" s="6"/>
+      <c r="B366" s="7"/>
     </row>
     <row r="367">
-      <c r="B367" s="6"/>
+      <c r="B367" s="7"/>
     </row>
     <row r="368">
-      <c r="B368" s="6"/>
+      <c r="B368" s="7"/>
     </row>
     <row r="369">
-      <c r="B369" s="6"/>
+      <c r="B369" s="7"/>
     </row>
     <row r="370">
-      <c r="B370" s="6"/>
+      <c r="B370" s="7"/>
     </row>
     <row r="371">
-      <c r="B371" s="6"/>
+      <c r="B371" s="7"/>
     </row>
     <row r="372">
-      <c r="B372" s="6"/>
+      <c r="B372" s="7"/>
     </row>
     <row r="373">
-      <c r="B373" s="6"/>
+      <c r="B373" s="7"/>
     </row>
     <row r="374">
-      <c r="B374" s="6"/>
+      <c r="B374" s="7"/>
     </row>
     <row r="375">
-      <c r="B375" s="6"/>
+      <c r="B375" s="7"/>
     </row>
     <row r="376">
-      <c r="B376" s="6"/>
+      <c r="B376" s="7"/>
     </row>
     <row r="377">
-      <c r="B377" s="6"/>
+      <c r="B377" s="7"/>
     </row>
     <row r="378">
-      <c r="B378" s="6"/>
+      <c r="B378" s="7"/>
     </row>
     <row r="379">
-      <c r="B379" s="6"/>
+      <c r="B379" s="7"/>
     </row>
     <row r="380">
-      <c r="B380" s="6"/>
+      <c r="B380" s="7"/>
     </row>
     <row r="381">
-      <c r="B381" s="6"/>
+      <c r="B381" s="7"/>
     </row>
     <row r="382">
-      <c r="B382" s="6"/>
+      <c r="B382" s="7"/>
     </row>
     <row r="383">
-      <c r="B383" s="6"/>
+      <c r="B383" s="7"/>
     </row>
     <row r="384">
-      <c r="B384" s="6"/>
+      <c r="B384" s="7"/>
     </row>
     <row r="385">
-      <c r="B385" s="6"/>
+      <c r="B385" s="7"/>
     </row>
     <row r="386">
-      <c r="B386" s="6"/>
+      <c r="B386" s="7"/>
     </row>
     <row r="387">
-      <c r="B387" s="6"/>
+      <c r="B387" s="7"/>
     </row>
     <row r="388">
-      <c r="B388" s="6"/>
+      <c r="B388" s="7"/>
     </row>
     <row r="389">
-      <c r="B389" s="6"/>
+      <c r="B389" s="7"/>
     </row>
     <row r="390">
-      <c r="B390" s="6"/>
+      <c r="B390" s="7"/>
     </row>
     <row r="391">
-      <c r="B391" s="6"/>
+      <c r="B391" s="7"/>
     </row>
     <row r="392">
-      <c r="B392" s="6"/>
+      <c r="B392" s="7"/>
     </row>
     <row r="393">
-      <c r="B393" s="6"/>
+      <c r="B393" s="7"/>
     </row>
     <row r="394">
-      <c r="B394" s="6"/>
+      <c r="B394" s="7"/>
     </row>
     <row r="395">
-      <c r="B395" s="6"/>
+      <c r="B395" s="7"/>
     </row>
     <row r="396">
-      <c r="B396" s="6"/>
+      <c r="B396" s="7"/>
     </row>
     <row r="397">
-      <c r="B397" s="6"/>
+      <c r="B397" s="7"/>
     </row>
     <row r="398">
-      <c r="B398" s="6"/>
+      <c r="B398" s="7"/>
     </row>
     <row r="399">
-      <c r="B399" s="6"/>
+      <c r="B399" s="7"/>
     </row>
     <row r="400">
-      <c r="B400" s="6"/>
+      <c r="B400" s="7"/>
     </row>
     <row r="401">
-      <c r="B401" s="6"/>
+      <c r="B401" s="7"/>
     </row>
     <row r="402">
-      <c r="B402" s="6"/>
+      <c r="B402" s="7"/>
     </row>
     <row r="403">
-      <c r="B403" s="6"/>
+      <c r="B403" s="7"/>
     </row>
     <row r="404">
-      <c r="B404" s="6"/>
+      <c r="B404" s="7"/>
     </row>
     <row r="405">
-      <c r="B405" s="6"/>
+      <c r="B405" s="7"/>
     </row>
     <row r="406">
-      <c r="B406" s="6"/>
+      <c r="B406" s="7"/>
     </row>
     <row r="407">
-      <c r="B407" s="6"/>
+      <c r="B407" s="7"/>
     </row>
     <row r="408">
-      <c r="B408" s="6"/>
+      <c r="B408" s="7"/>
     </row>
     <row r="409">
-      <c r="B409" s="6"/>
+      <c r="B409" s="7"/>
     </row>
     <row r="410">
-      <c r="B410" s="6"/>
+      <c r="B410" s="7"/>
     </row>
     <row r="411">
-      <c r="B411" s="6"/>
+      <c r="B411" s="7"/>
     </row>
     <row r="412">
-      <c r="B412" s="6"/>
+      <c r="B412" s="7"/>
     </row>
     <row r="413">
-      <c r="B413" s="6"/>
+      <c r="B413" s="7"/>
     </row>
     <row r="414">
-      <c r="B414" s="6"/>
+      <c r="B414" s="7"/>
     </row>
     <row r="415">
-      <c r="B415" s="6"/>
+      <c r="B415" s="7"/>
     </row>
     <row r="416">
-      <c r="B416" s="6"/>
+      <c r="B416" s="7"/>
     </row>
     <row r="417">
-      <c r="B417" s="6"/>
+      <c r="B417" s="7"/>
     </row>
     <row r="418">
-      <c r="B418" s="6"/>
+      <c r="B418" s="7"/>
     </row>
     <row r="419">
-      <c r="B419" s="6"/>
+      <c r="B419" s="7"/>
     </row>
     <row r="420">
-      <c r="B420" s="6"/>
+      <c r="B420" s="7"/>
     </row>
     <row r="421">
-      <c r="B421" s="6"/>
+      <c r="B421" s="7"/>
     </row>
     <row r="422">
-      <c r="B422" s="6"/>
+      <c r="B422" s="7"/>
     </row>
     <row r="423">
-      <c r="B423" s="6"/>
+      <c r="B423" s="7"/>
     </row>
     <row r="424">
-      <c r="B424" s="6"/>
+      <c r="B424" s="7"/>
     </row>
     <row r="425">
-      <c r="B425" s="6"/>
+      <c r="B425" s="7"/>
     </row>
     <row r="426">
-      <c r="B426" s="6"/>
+      <c r="B426" s="7"/>
     </row>
     <row r="427">
-      <c r="B427" s="6"/>
+      <c r="B427" s="7"/>
     </row>
     <row r="428">
-      <c r="B428" s="6"/>
+      <c r="B428" s="7"/>
     </row>
     <row r="429">
-      <c r="B429" s="6"/>
+      <c r="B429" s="7"/>
     </row>
     <row r="430">
-      <c r="B430" s="6"/>
+      <c r="B430" s="7"/>
     </row>
     <row r="431">
-      <c r="B431" s="6"/>
+      <c r="B431" s="7"/>
     </row>
     <row r="432">
-      <c r="B432" s="6"/>
+      <c r="B432" s="7"/>
     </row>
     <row r="433">
-      <c r="B433" s="6"/>
+      <c r="B433" s="7"/>
     </row>
     <row r="434">
-      <c r="B434" s="6"/>
+      <c r="B434" s="7"/>
     </row>
     <row r="435">
-      <c r="B435" s="6"/>
+      <c r="B435" s="7"/>
     </row>
     <row r="436">
-      <c r="B436" s="6"/>
+      <c r="B436" s="7"/>
     </row>
     <row r="437">
-      <c r="B437" s="6"/>
+      <c r="B437" s="7"/>
     </row>
     <row r="438">
-      <c r="B438" s="6"/>
+      <c r="B438" s="7"/>
     </row>
     <row r="439">
-      <c r="B439" s="6"/>
+      <c r="B439" s="7"/>
     </row>
     <row r="440">
-      <c r="B440" s="6"/>
+      <c r="B440" s="7"/>
     </row>
     <row r="441">
-      <c r="B441" s="6"/>
+      <c r="B441" s="7"/>
     </row>
     <row r="442">
-      <c r="B442" s="6"/>
+      <c r="B442" s="7"/>
     </row>
     <row r="443">
-      <c r="B443" s="6"/>
+      <c r="B443" s="7"/>
     </row>
     <row r="444">
-      <c r="B444" s="6"/>
+      <c r="B444" s="7"/>
     </row>
     <row r="445">
-      <c r="B445" s="6"/>
+      <c r="B445" s="7"/>
     </row>
     <row r="446">
-      <c r="B446" s="6"/>
+      <c r="B446" s="7"/>
     </row>
     <row r="447">
-      <c r="B447" s="6"/>
+      <c r="B447" s="7"/>
     </row>
     <row r="448">
-      <c r="B448" s="6"/>
+      <c r="B448" s="7"/>
     </row>
     <row r="449">
-      <c r="B449" s="6"/>
+      <c r="B449" s="7"/>
     </row>
     <row r="450">
-      <c r="B450" s="6"/>
+      <c r="B450" s="7"/>
     </row>
     <row r="451">
-      <c r="B451" s="6"/>
+      <c r="B451" s="7"/>
     </row>
     <row r="452">
-      <c r="B452" s="6"/>
+      <c r="B452" s="7"/>
     </row>
     <row r="453">
-      <c r="B453" s="6"/>
+      <c r="B453" s="7"/>
     </row>
     <row r="454">
-      <c r="B454" s="6"/>
+      <c r="B454" s="7"/>
     </row>
     <row r="455">
-      <c r="B455" s="6"/>
+      <c r="B455" s="7"/>
     </row>
     <row r="456">
-      <c r="B456" s="6"/>
+      <c r="B456" s="7"/>
     </row>
     <row r="457">
-      <c r="B457" s="6"/>
+      <c r="B457" s="7"/>
     </row>
     <row r="458">
-      <c r="B458" s="6"/>
+      <c r="B458" s="7"/>
     </row>
     <row r="459">
-      <c r="B459" s="6"/>
+      <c r="B459" s="7"/>
     </row>
     <row r="460">
-      <c r="B460" s="6"/>
+      <c r="B460" s="7"/>
     </row>
     <row r="461">
-      <c r="B461" s="6"/>
+      <c r="B461" s="7"/>
     </row>
     <row r="462">
-      <c r="B462" s="6"/>
+      <c r="B462" s="7"/>
     </row>
     <row r="463">
-      <c r="B463" s="6"/>
+      <c r="B463" s="7"/>
     </row>
     <row r="464">
-      <c r="B464" s="6"/>
+      <c r="B464" s="7"/>
     </row>
     <row r="465">
-      <c r="B465" s="6"/>
+      <c r="B465" s="7"/>
     </row>
     <row r="466">
-      <c r="B466" s="6"/>
+      <c r="B466" s="7"/>
     </row>
     <row r="467">
-      <c r="B467" s="6"/>
+      <c r="B467" s="7"/>
     </row>
     <row r="468">
-      <c r="B468" s="6"/>
+      <c r="B468" s="7"/>
     </row>
     <row r="469">
-      <c r="B469" s="6"/>
+      <c r="B469" s="7"/>
     </row>
     <row r="470">
-      <c r="B470" s="6"/>
+      <c r="B470" s="7"/>
     </row>
     <row r="471">
-      <c r="B471" s="6"/>
+      <c r="B471" s="7"/>
     </row>
     <row r="472">
-      <c r="B472" s="6"/>
+      <c r="B472" s="7"/>
     </row>
     <row r="473">
-      <c r="B473" s="6"/>
+      <c r="B473" s="7"/>
     </row>
     <row r="474">
-      <c r="B474" s="6"/>
+      <c r="B474" s="7"/>
     </row>
     <row r="475">
-      <c r="B475" s="6"/>
+      <c r="B475" s="7"/>
     </row>
     <row r="476">
-      <c r="B476" s="6"/>
+      <c r="B476" s="7"/>
     </row>
     <row r="477">
-      <c r="B477" s="6"/>
+      <c r="B477" s="7"/>
     </row>
     <row r="478">
-      <c r="B478" s="6"/>
+      <c r="B478" s="7"/>
     </row>
     <row r="479">
-      <c r="B479" s="6"/>
+      <c r="B479" s="7"/>
     </row>
     <row r="480">
-      <c r="B480" s="6"/>
+      <c r="B480" s="7"/>
     </row>
     <row r="481">
-      <c r="B481" s="6"/>
+      <c r="B481" s="7"/>
     </row>
     <row r="482">
-      <c r="B482" s="6"/>
+      <c r="B482" s="7"/>
     </row>
     <row r="483">
-      <c r="B483" s="6"/>
+      <c r="B483" s="7"/>
     </row>
     <row r="484">
-      <c r="B484" s="6"/>
+      <c r="B484" s="7"/>
     </row>
     <row r="485">
-      <c r="B485" s="6"/>
+      <c r="B485" s="7"/>
     </row>
     <row r="486">
-      <c r="B486" s="6"/>
+      <c r="B486" s="7"/>
     </row>
     <row r="487">
-      <c r="B487" s="6"/>
+      <c r="B487" s="7"/>
     </row>
     <row r="488">
-      <c r="B488" s="6"/>
+      <c r="B488" s="7"/>
     </row>
     <row r="489">
-      <c r="B489" s="6"/>
+      <c r="B489" s="7"/>
     </row>
     <row r="490">
-      <c r="B490" s="6"/>
+      <c r="B490" s="7"/>
     </row>
     <row r="491">
-      <c r="B491" s="6"/>
+      <c r="B491" s="7"/>
     </row>
     <row r="492">
-      <c r="B492" s="6"/>
+      <c r="B492" s="7"/>
     </row>
     <row r="493">
-      <c r="B493" s="6"/>
+      <c r="B493" s="7"/>
     </row>
     <row r="494">
-      <c r="B494" s="6"/>
+      <c r="B494" s="7"/>
     </row>
     <row r="495">
-      <c r="B495" s="6"/>
+      <c r="B495" s="7"/>
     </row>
     <row r="496">
-      <c r="B496" s="6"/>
+      <c r="B496" s="7"/>
     </row>
     <row r="497">
-      <c r="B497" s="6"/>
+      <c r="B497" s="7"/>
     </row>
     <row r="498">
-      <c r="B498" s="6"/>
+      <c r="B498" s="7"/>
     </row>
     <row r="499">
-      <c r="B499" s="6"/>
+      <c r="B499" s="7"/>
     </row>
     <row r="500">
-      <c r="B500" s="6"/>
+      <c r="B500" s="7"/>
     </row>
     <row r="501">
-      <c r="B501" s="6"/>
+      <c r="B501" s="7"/>
     </row>
     <row r="502">
-      <c r="B502" s="6"/>
+      <c r="B502" s="7"/>
     </row>
     <row r="503">
-      <c r="B503" s="6"/>
+      <c r="B503" s="7"/>
     </row>
     <row r="504">
-      <c r="B504" s="6"/>
+      <c r="B504" s="7"/>
     </row>
     <row r="505">
-      <c r="B505" s="6"/>
+      <c r="B505" s="7"/>
     </row>
     <row r="506">
-      <c r="B506" s="6"/>
+      <c r="B506" s="7"/>
     </row>
     <row r="507">
-      <c r="B507" s="6"/>
+      <c r="B507" s="7"/>
     </row>
     <row r="508">
-      <c r="B508" s="6"/>
+      <c r="B508" s="7"/>
     </row>
     <row r="509">
-      <c r="B509" s="6"/>
+      <c r="B509" s="7"/>
     </row>
     <row r="510">
-      <c r="B510" s="6"/>
+      <c r="B510" s="7"/>
     </row>
     <row r="511">
-      <c r="B511" s="6"/>
+      <c r="B511" s="7"/>
     </row>
     <row r="512">
-      <c r="B512" s="6"/>
+      <c r="B512" s="7"/>
     </row>
     <row r="513">
-      <c r="B513" s="6"/>
+      <c r="B513" s="7"/>
     </row>
     <row r="514">
-      <c r="B514" s="6"/>
+      <c r="B514" s="7"/>
     </row>
     <row r="515">
-      <c r="B515" s="6"/>
+      <c r="B515" s="7"/>
     </row>
     <row r="516">
-      <c r="B516" s="6"/>
+      <c r="B516" s="7"/>
     </row>
     <row r="517">
-      <c r="B517" s="6"/>
+      <c r="B517" s="7"/>
     </row>
     <row r="518">
-      <c r="B518" s="6"/>
+      <c r="B518" s="7"/>
     </row>
     <row r="519">
-      <c r="B519" s="6"/>
+      <c r="B519" s="7"/>
     </row>
     <row r="520">
-      <c r="B520" s="6"/>
+      <c r="B520" s="7"/>
     </row>
     <row r="521">
-      <c r="B521" s="6"/>
+      <c r="B521" s="7"/>
     </row>
     <row r="522">
-      <c r="B522" s="6"/>
+      <c r="B522" s="7"/>
     </row>
     <row r="523">
-      <c r="B523" s="6"/>
+      <c r="B523" s="7"/>
     </row>
     <row r="524">
-      <c r="B524" s="6"/>
+      <c r="B524" s="7"/>
     </row>
     <row r="525">
-      <c r="B525" s="6"/>
+      <c r="B525" s="7"/>
     </row>
     <row r="526">
-      <c r="B526" s="6"/>
+      <c r="B526" s="7"/>
     </row>
     <row r="527">
-      <c r="B527" s="6"/>
+      <c r="B527" s="7"/>
     </row>
     <row r="528">
-      <c r="B528" s="6"/>
+      <c r="B528" s="7"/>
     </row>
     <row r="529">
-      <c r="B529" s="6"/>
+      <c r="B529" s="7"/>
     </row>
     <row r="530">
-      <c r="B530" s="6"/>
+      <c r="B530" s="7"/>
     </row>
     <row r="531">
-      <c r="B531" s="6"/>
+      <c r="B531" s="7"/>
     </row>
     <row r="532">
-      <c r="B532" s="6"/>
+      <c r="B532" s="7"/>
     </row>
     <row r="533">
-      <c r="B533" s="6"/>
+      <c r="B533" s="7"/>
     </row>
     <row r="534">
-      <c r="B534" s="6"/>
+      <c r="B534" s="7"/>
     </row>
     <row r="535">
-      <c r="B535" s="6"/>
+      <c r="B535" s="7"/>
     </row>
     <row r="536">
-      <c r="B536" s="6"/>
+      <c r="B536" s="7"/>
     </row>
     <row r="537">
-      <c r="B537" s="6"/>
+      <c r="B537" s="7"/>
     </row>
     <row r="538">
-      <c r="B538" s="6"/>
+      <c r="B538" s="7"/>
     </row>
     <row r="539">
-      <c r="B539" s="6"/>
+      <c r="B539" s="7"/>
     </row>
     <row r="540">
-      <c r="B540" s="6"/>
+      <c r="B540" s="7"/>
     </row>
     <row r="541">
-      <c r="B541" s="6"/>
+      <c r="B541" s="7"/>
     </row>
     <row r="542">
-      <c r="B542" s="6"/>
+      <c r="B542" s="7"/>
     </row>
     <row r="543">
-      <c r="B543" s="6"/>
+      <c r="B543" s="7"/>
     </row>
     <row r="544">
-      <c r="B544" s="6"/>
+      <c r="B544" s="7"/>
     </row>
     <row r="545">
-      <c r="B545" s="6"/>
+      <c r="B545" s="7"/>
     </row>
     <row r="546">
-      <c r="B546" s="6"/>
+      <c r="B546" s="7"/>
     </row>
     <row r="547">
-      <c r="B547" s="6"/>
+      <c r="B547" s="7"/>
     </row>
     <row r="548">
-      <c r="B548" s="6"/>
+      <c r="B548" s="7"/>
     </row>
     <row r="549">
-      <c r="B549" s="6"/>
+      <c r="B549" s="7"/>
     </row>
     <row r="550">
-      <c r="B550" s="6"/>
+      <c r="B550" s="7"/>
     </row>
     <row r="551">
-      <c r="B551" s="6"/>
+      <c r="B551" s="7"/>
     </row>
     <row r="552">
-      <c r="B552" s="6"/>
+      <c r="B552" s="7"/>
     </row>
     <row r="553">
-      <c r="B553" s="6"/>
+      <c r="B553" s="7"/>
     </row>
     <row r="554">
-      <c r="B554" s="6"/>
+      <c r="B554" s="7"/>
     </row>
     <row r="555">
-      <c r="B555" s="6"/>
+      <c r="B555" s="7"/>
     </row>
     <row r="556">
-      <c r="B556" s="6"/>
+      <c r="B556" s="7"/>
     </row>
     <row r="557">
-      <c r="B557" s="6"/>
+      <c r="B557" s="7"/>
     </row>
     <row r="558">
-      <c r="B558" s="6"/>
+      <c r="B558" s="7"/>
     </row>
     <row r="559">
-      <c r="B559" s="6"/>
+      <c r="B559" s="7"/>
     </row>
     <row r="560">
-      <c r="B560" s="6"/>
+      <c r="B560" s="7"/>
     </row>
     <row r="561">
-      <c r="B561" s="6"/>
+      <c r="B561" s="7"/>
     </row>
     <row r="562">
-      <c r="B562" s="6"/>
+      <c r="B562" s="7"/>
     </row>
     <row r="563">
-      <c r="B563" s="6"/>
+      <c r="B563" s="7"/>
     </row>
     <row r="564">
-      <c r="B564" s="6"/>
+      <c r="B564" s="7"/>
     </row>
     <row r="565">
-      <c r="B565" s="6"/>
+      <c r="B565" s="7"/>
     </row>
     <row r="566">
-      <c r="B566" s="6"/>
+      <c r="B566" s="7"/>
     </row>
     <row r="567">
-      <c r="B567" s="6"/>
+      <c r="B567" s="7"/>
     </row>
     <row r="568">
-      <c r="B568" s="6"/>
+      <c r="B568" s="7"/>
     </row>
     <row r="569">
-      <c r="B569" s="6"/>
+      <c r="B569" s="7"/>
     </row>
     <row r="570">
-      <c r="B570" s="6"/>
+      <c r="B570" s="7"/>
     </row>
     <row r="571">
-      <c r="B571" s="6"/>
+      <c r="B571" s="7"/>
     </row>
     <row r="572">
-      <c r="B572" s="6"/>
+      <c r="B572" s="7"/>
     </row>
     <row r="573">
-      <c r="B573" s="6"/>
+      <c r="B573" s="7"/>
     </row>
     <row r="574">
-      <c r="B574" s="6"/>
+      <c r="B574" s="7"/>
     </row>
     <row r="575">
-      <c r="B575" s="6"/>
+      <c r="B575" s="7"/>
     </row>
     <row r="576">
-      <c r="B576" s="6"/>
+      <c r="B576" s="7"/>
     </row>
     <row r="577">
-      <c r="B577" s="6"/>
+      <c r="B577" s="7"/>
     </row>
     <row r="578">
-      <c r="B578" s="6"/>
+      <c r="B578" s="7"/>
     </row>
     <row r="579">
-      <c r="B579" s="6"/>
+      <c r="B579" s="7"/>
     </row>
     <row r="580">
-      <c r="B580" s="6"/>
+      <c r="B580" s="7"/>
     </row>
     <row r="581">
-      <c r="B581" s="6"/>
+      <c r="B581" s="7"/>
     </row>
     <row r="582">
-      <c r="B582" s="6"/>
+      <c r="B582" s="7"/>
     </row>
     <row r="583">
-      <c r="B583" s="6"/>
+      <c r="B583" s="7"/>
     </row>
     <row r="584">
-      <c r="B584" s="6"/>
+      <c r="B584" s="7"/>
     </row>
     <row r="585">
-      <c r="B585" s="6"/>
+      <c r="B585" s="7"/>
     </row>
     <row r="586">
-      <c r="B586" s="6"/>
+      <c r="B586" s="7"/>
     </row>
     <row r="587">
-      <c r="B587" s="6"/>
+      <c r="B587" s="7"/>
     </row>
     <row r="588">
-      <c r="B588" s="6"/>
+      <c r="B588" s="7"/>
     </row>
     <row r="589">
-      <c r="B589" s="6"/>
+      <c r="B589" s="7"/>
     </row>
     <row r="590">
-      <c r="B590" s="6"/>
+      <c r="B590" s="7"/>
     </row>
     <row r="591">
-      <c r="B591" s="6"/>
+      <c r="B591" s="7"/>
     </row>
     <row r="592">
-      <c r="B592" s="6"/>
+      <c r="B592" s="7"/>
     </row>
     <row r="593">
-      <c r="B593" s="6"/>
+      <c r="B593" s="7"/>
     </row>
     <row r="594">
-      <c r="B594" s="6"/>
+      <c r="B594" s="7"/>
     </row>
     <row r="595">
-      <c r="B595" s="6"/>
+      <c r="B595" s="7"/>
     </row>
     <row r="596">
-      <c r="B596" s="6"/>
+      <c r="B596" s="7"/>
     </row>
     <row r="597">
-      <c r="B597" s="6"/>
+      <c r="B597" s="7"/>
     </row>
     <row r="598">
-      <c r="B598" s="6"/>
+      <c r="B598" s="7"/>
     </row>
     <row r="599">
-      <c r="B599" s="6"/>
+      <c r="B599" s="7"/>
     </row>
     <row r="600">
-      <c r="B600" s="6"/>
+      <c r="B600" s="7"/>
     </row>
     <row r="601">
-      <c r="B601" s="6"/>
+      <c r="B601" s="7"/>
     </row>
     <row r="602">
-      <c r="B602" s="6"/>
+      <c r="B602" s="7"/>
     </row>
     <row r="603">
-      <c r="B603" s="6"/>
+      <c r="B603" s="7"/>
     </row>
     <row r="604">
-      <c r="B604" s="6"/>
+      <c r="B604" s="7"/>
     </row>
     <row r="605">
-      <c r="B605" s="6"/>
+      <c r="B605" s="7"/>
     </row>
     <row r="606">
-      <c r="B606" s="6"/>
+      <c r="B606" s="7"/>
     </row>
     <row r="607">
-      <c r="B607" s="6"/>
+      <c r="B607" s="7"/>
     </row>
     <row r="608">
-      <c r="B608" s="6"/>
+      <c r="B608" s="7"/>
     </row>
     <row r="609">
-      <c r="B609" s="6"/>
+      <c r="B609" s="7"/>
     </row>
     <row r="610">
-      <c r="B610" s="6"/>
+      <c r="B610" s="7"/>
     </row>
     <row r="611">
-      <c r="B611" s="6"/>
+      <c r="B611" s="7"/>
     </row>
     <row r="612">
-      <c r="B612" s="6"/>
+      <c r="B612" s="7"/>
     </row>
     <row r="613">
-      <c r="B613" s="6"/>
+      <c r="B613" s="7"/>
     </row>
     <row r="614">
-      <c r="B614" s="6"/>
+      <c r="B614" s="7"/>
     </row>
     <row r="615">
-      <c r="B615" s="6"/>
+      <c r="B615" s="7"/>
     </row>
     <row r="616">
-      <c r="B616" s="6"/>
+      <c r="B616" s="7"/>
     </row>
     <row r="617">
-      <c r="B617" s="6"/>
+      <c r="B617" s="7"/>
     </row>
     <row r="618">
-      <c r="B618" s="6"/>
+      <c r="B618" s="7"/>
     </row>
     <row r="619">
-      <c r="B619" s="6"/>
+      <c r="B619" s="7"/>
     </row>
     <row r="620">
-      <c r="B620" s="6"/>
+      <c r="B620" s="7"/>
     </row>
     <row r="621">
-      <c r="B621" s="6"/>
+      <c r="B621" s="7"/>
     </row>
     <row r="622">
-      <c r="B622" s="6"/>
+      <c r="B622" s="7"/>
     </row>
     <row r="623">
-      <c r="B623" s="6"/>
+      <c r="B623" s="7"/>
     </row>
     <row r="624">
-      <c r="B624" s="6"/>
+      <c r="B624" s="7"/>
     </row>
     <row r="625">
-      <c r="B625" s="6"/>
+      <c r="B625" s="7"/>
     </row>
     <row r="626">
-      <c r="B626" s="6"/>
+      <c r="B626" s="7"/>
     </row>
     <row r="627">
-      <c r="B627" s="6"/>
+      <c r="B627" s="7"/>
     </row>
     <row r="628">
-      <c r="B628" s="6"/>
+      <c r="B628" s="7"/>
     </row>
     <row r="629">
-      <c r="B629" s="6"/>
+      <c r="B629" s="7"/>
     </row>
     <row r="630">
-      <c r="B630" s="6"/>
+      <c r="B630" s="7"/>
     </row>
     <row r="631">
-      <c r="B631" s="6"/>
+      <c r="B631" s="7"/>
     </row>
     <row r="632">
-      <c r="B632" s="6"/>
+      <c r="B632" s="7"/>
     </row>
     <row r="633">
-      <c r="B633" s="6"/>
+      <c r="B633" s="7"/>
     </row>
     <row r="634">
-      <c r="B634" s="6"/>
+      <c r="B634" s="7"/>
     </row>
     <row r="635">
-      <c r="B635" s="6"/>
+      <c r="B635" s="7"/>
     </row>
     <row r="636">
-      <c r="B636" s="6"/>
+      <c r="B636" s="7"/>
     </row>
     <row r="637">
-      <c r="B637" s="6"/>
+      <c r="B637" s="7"/>
     </row>
     <row r="638">
-      <c r="B638" s="6"/>
+      <c r="B638" s="7"/>
     </row>
     <row r="639">
-      <c r="B639" s="6"/>
+      <c r="B639" s="7"/>
     </row>
     <row r="640">
-      <c r="B640" s="6"/>
+      <c r="B640" s="7"/>
     </row>
     <row r="641">
-      <c r="B641" s="6"/>
+      <c r="B641" s="7"/>
     </row>
     <row r="642">
-      <c r="B642" s="6"/>
+      <c r="B642" s="7"/>
     </row>
     <row r="643">
-      <c r="B643" s="6"/>
+      <c r="B643" s="7"/>
     </row>
     <row r="644">
-      <c r="B644" s="6"/>
+      <c r="B644" s="7"/>
     </row>
     <row r="645">
-      <c r="B645" s="6"/>
+      <c r="B645" s="7"/>
     </row>
     <row r="646">
-      <c r="B646" s="6"/>
+      <c r="B646" s="7"/>
     </row>
     <row r="647">
-      <c r="B647" s="6"/>
+      <c r="B647" s="7"/>
     </row>
     <row r="648">
-      <c r="B648" s="6"/>
+      <c r="B648" s="7"/>
     </row>
     <row r="649">
-      <c r="B649" s="6"/>
+      <c r="B649" s="7"/>
     </row>
     <row r="650">
-      <c r="B650" s="6"/>
+      <c r="B650" s="7"/>
     </row>
     <row r="651">
-      <c r="B651" s="6"/>
+      <c r="B651" s="7"/>
     </row>
     <row r="652">
-      <c r="B652" s="6"/>
+      <c r="B652" s="7"/>
     </row>
     <row r="653">
-      <c r="B653" s="6"/>
+      <c r="B653" s="7"/>
     </row>
     <row r="654">
-      <c r="B654" s="6"/>
+      <c r="B654" s="7"/>
     </row>
     <row r="655">
-      <c r="B655" s="6"/>
+      <c r="B655" s="7"/>
     </row>
     <row r="656">
-      <c r="B656" s="6"/>
+      <c r="B656" s="7"/>
     </row>
     <row r="657">
-      <c r="B657" s="6"/>
+      <c r="B657" s="7"/>
     </row>
     <row r="658">
-      <c r="B658" s="6"/>
+      <c r="B658" s="7"/>
     </row>
     <row r="659">
-      <c r="B659" s="6"/>
+      <c r="B659" s="7"/>
     </row>
     <row r="660">
-      <c r="B660" s="6"/>
+      <c r="B660" s="7"/>
     </row>
     <row r="661">
-      <c r="B661" s="6"/>
+      <c r="B661" s="7"/>
     </row>
     <row r="662">
-      <c r="B662" s="6"/>
+      <c r="B662" s="7"/>
     </row>
     <row r="663">
-      <c r="B663" s="6"/>
+      <c r="B663" s="7"/>
     </row>
     <row r="664">
-      <c r="B664" s="6"/>
+      <c r="B664" s="7"/>
     </row>
     <row r="665">
-      <c r="B665" s="6"/>
+      <c r="B665" s="7"/>
     </row>
     <row r="666">
-      <c r="B666" s="6"/>
+      <c r="B666" s="7"/>
     </row>
     <row r="667">
-      <c r="B667" s="6"/>
+      <c r="B667" s="7"/>
     </row>
     <row r="668">
-      <c r="B668" s="6"/>
+      <c r="B668" s="7"/>
     </row>
     <row r="669">
-      <c r="B669" s="6"/>
+      <c r="B669" s="7"/>
     </row>
     <row r="670">
-      <c r="B670" s="6"/>
+      <c r="B670" s="7"/>
     </row>
     <row r="671">
-      <c r="B671" s="6"/>
+      <c r="B671" s="7"/>
     </row>
     <row r="672">
-      <c r="B672" s="6"/>
+      <c r="B672" s="7"/>
     </row>
     <row r="673">
-      <c r="B673" s="6"/>
+      <c r="B673" s="7"/>
     </row>
     <row r="674">
-      <c r="B674" s="6"/>
+      <c r="B674" s="7"/>
     </row>
     <row r="675">
-      <c r="B675" s="6"/>
+      <c r="B675" s="7"/>
     </row>
     <row r="676">
-      <c r="B676" s="6"/>
+      <c r="B676" s="7"/>
     </row>
     <row r="677">
-      <c r="B677" s="6"/>
+      <c r="B677" s="7"/>
     </row>
     <row r="678">
-      <c r="B678" s="6"/>
+      <c r="B678" s="7"/>
     </row>
     <row r="679">
-      <c r="B679" s="6"/>
+      <c r="B679" s="7"/>
     </row>
     <row r="680">
-      <c r="B680" s="6"/>
+      <c r="B680" s="7"/>
     </row>
     <row r="681">
-      <c r="B681" s="6"/>
+      <c r="B681" s="7"/>
     </row>
     <row r="682">
-      <c r="B682" s="6"/>
+      <c r="B682" s="7"/>
     </row>
     <row r="683">
-      <c r="B683" s="6"/>
+      <c r="B683" s="7"/>
     </row>
     <row r="684">
-      <c r="B684" s="6"/>
+      <c r="B684" s="7"/>
     </row>
     <row r="685">
-      <c r="B685" s="6"/>
+      <c r="B685" s="7"/>
     </row>
     <row r="686">
-      <c r="B686" s="6"/>
+      <c r="B686" s="7"/>
     </row>
     <row r="687">
-      <c r="B687" s="6"/>
+      <c r="B687" s="7"/>
     </row>
     <row r="688">
-      <c r="B688" s="6"/>
+      <c r="B688" s="7"/>
     </row>
     <row r="689">
-      <c r="B689" s="6"/>
+      <c r="B689" s="7"/>
     </row>
     <row r="690">
-      <c r="B690" s="6"/>
+      <c r="B690" s="7"/>
     </row>
     <row r="691">
-      <c r="B691" s="6"/>
+      <c r="B691" s="7"/>
     </row>
     <row r="692">
-      <c r="B692" s="6"/>
+      <c r="B692" s="7"/>
     </row>
     <row r="693">
-      <c r="B693" s="6"/>
+      <c r="B693" s="7"/>
     </row>
     <row r="694">
-      <c r="B694" s="6"/>
+      <c r="B694" s="7"/>
     </row>
     <row r="695">
-      <c r="B695" s="6"/>
+      <c r="B695" s="7"/>
     </row>
     <row r="696">
-      <c r="B696" s="6"/>
+      <c r="B696" s="7"/>
     </row>
     <row r="697">
-      <c r="B697" s="6"/>
+      <c r="B697" s="7"/>
     </row>
     <row r="698">
-      <c r="B698" s="6"/>
+      <c r="B698" s="7"/>
     </row>
     <row r="699">
-      <c r="B699" s="6"/>
+      <c r="B699" s="7"/>
     </row>
     <row r="700">
-      <c r="B700" s="6"/>
+      <c r="B700" s="7"/>
     </row>
     <row r="701">
-      <c r="B701" s="6"/>
+      <c r="B701" s="7"/>
     </row>
     <row r="702">
-      <c r="B702" s="6"/>
+      <c r="B702" s="7"/>
     </row>
     <row r="703">
-      <c r="B703" s="6"/>
+      <c r="B703" s="7"/>
     </row>
     <row r="704">
-      <c r="B704" s="6"/>
+      <c r="B704" s="7"/>
     </row>
     <row r="705">
-      <c r="B705" s="6"/>
+      <c r="B705" s="7"/>
     </row>
     <row r="706">
-      <c r="B706" s="6"/>
+      <c r="B706" s="7"/>
     </row>
     <row r="707">
-      <c r="B707" s="6"/>
+      <c r="B707" s="7"/>
     </row>
     <row r="708">
-      <c r="B708" s="6"/>
+      <c r="B708" s="7"/>
     </row>
     <row r="709">
-      <c r="B709" s="6"/>
+      <c r="B709" s="7"/>
     </row>
     <row r="710">
-      <c r="B710" s="6"/>
+      <c r="B710" s="7"/>
     </row>
     <row r="711">
-      <c r="B711" s="6"/>
+      <c r="B711" s="7"/>
     </row>
     <row r="712">
-      <c r="B712" s="6"/>
+      <c r="B712" s="7"/>
     </row>
     <row r="713">
-      <c r="B713" s="6"/>
+      <c r="B713" s="7"/>
     </row>
     <row r="714">
-      <c r="B714" s="6"/>
+      <c r="B714" s="7"/>
     </row>
     <row r="715">
-      <c r="B715" s="6"/>
+      <c r="B715" s="7"/>
     </row>
     <row r="716">
-      <c r="B716" s="6"/>
+      <c r="B716" s="7"/>
     </row>
     <row r="717">
-      <c r="B717" s="6"/>
+      <c r="B717" s="7"/>
     </row>
     <row r="718">
-      <c r="B718" s="6"/>
+      <c r="B718" s="7"/>
     </row>
     <row r="719">
-      <c r="B719" s="6"/>
+      <c r="B719" s="7"/>
     </row>
     <row r="720">
-      <c r="B720" s="6"/>
+      <c r="B720" s="7"/>
     </row>
     <row r="721">
-      <c r="B721" s="6"/>
+      <c r="B721" s="7"/>
     </row>
     <row r="722">
-      <c r="B722" s="6"/>
+      <c r="B722" s="7"/>
     </row>
     <row r="723">
-      <c r="B723" s="6"/>
+      <c r="B723" s="7"/>
     </row>
     <row r="724">
-      <c r="B724" s="6"/>
+      <c r="B724" s="7"/>
     </row>
     <row r="725">
-      <c r="B725" s="6"/>
+      <c r="B725" s="7"/>
     </row>
     <row r="726">
-      <c r="B726" s="6"/>
+      <c r="B726" s="7"/>
     </row>
     <row r="727">
-      <c r="B727" s="6"/>
+      <c r="B727" s="7"/>
     </row>
     <row r="728">
-      <c r="B728" s="6"/>
+      <c r="B728" s="7"/>
     </row>
     <row r="729">
-      <c r="B729" s="6"/>
+      <c r="B729" s="7"/>
     </row>
     <row r="730">
-      <c r="B730" s="6"/>
+      <c r="B730" s="7"/>
     </row>
     <row r="731">
-      <c r="B731" s="6"/>
+      <c r="B731" s="7"/>
     </row>
     <row r="732">
-      <c r="B732" s="6"/>
+      <c r="B732" s="7"/>
     </row>
     <row r="733">
-      <c r="B733" s="6"/>
+      <c r="B733" s="7"/>
     </row>
     <row r="734">
-      <c r="B734" s="6"/>
+      <c r="B734" s="7"/>
     </row>
     <row r="735">
-      <c r="B735" s="6"/>
+      <c r="B735" s="7"/>
     </row>
     <row r="736">
-      <c r="B736" s="6"/>
+      <c r="B736" s="7"/>
     </row>
     <row r="737">
-      <c r="B737" s="6"/>
+      <c r="B737" s="7"/>
     </row>
     <row r="738">
-      <c r="B738" s="6"/>
+      <c r="B738" s="7"/>
     </row>
     <row r="739">
-      <c r="B739" s="6"/>
+      <c r="B739" s="7"/>
     </row>
     <row r="740">
-      <c r="B740" s="6"/>
+      <c r="B740" s="7"/>
     </row>
     <row r="741">
-      <c r="B741" s="6"/>
+      <c r="B741" s="7"/>
     </row>
     <row r="742">
-      <c r="B742" s="6"/>
+      <c r="B742" s="7"/>
     </row>
     <row r="743">
-      <c r="B743" s="6"/>
+      <c r="B743" s="7"/>
     </row>
     <row r="744">
-      <c r="B744" s="6"/>
+      <c r="B744" s="7"/>
     </row>
     <row r="745">
-      <c r="B745" s="6"/>
+      <c r="B745" s="7"/>
     </row>
     <row r="746">
-      <c r="B746" s="6"/>
+      <c r="B746" s="7"/>
     </row>
     <row r="747">
-      <c r="B747" s="6"/>
+      <c r="B747" s="7"/>
     </row>
     <row r="748">
-      <c r="B748" s="6"/>
+      <c r="B748" s="7"/>
     </row>
     <row r="749">
-      <c r="B749" s="6"/>
+      <c r="B749" s="7"/>
     </row>
     <row r="750">
-      <c r="B750" s="6"/>
+      <c r="B750" s="7"/>
     </row>
     <row r="751">
-      <c r="B751" s="6"/>
+      <c r="B751" s="7"/>
     </row>
     <row r="752">
-      <c r="B752" s="6"/>
+      <c r="B752" s="7"/>
     </row>
     <row r="753">
-      <c r="B753" s="6"/>
+      <c r="B753" s="7"/>
     </row>
     <row r="754">
-      <c r="B754" s="6"/>
+      <c r="B754" s="7"/>
     </row>
     <row r="755">
-      <c r="B755" s="6"/>
+      <c r="B755" s="7"/>
     </row>
     <row r="756">
-      <c r="B756" s="6"/>
+      <c r="B756" s="7"/>
     </row>
     <row r="757">
-      <c r="B757" s="6"/>
+      <c r="B757" s="7"/>
     </row>
     <row r="758">
-      <c r="B758" s="6"/>
+      <c r="B758" s="7"/>
     </row>
     <row r="759">
-      <c r="B759" s="6"/>
+      <c r="B759" s="7"/>
     </row>
     <row r="760">
-      <c r="B760" s="6"/>
+      <c r="B760" s="7"/>
     </row>
     <row r="761">
-      <c r="B761" s="6"/>
+      <c r="B761" s="7"/>
     </row>
     <row r="762">
-      <c r="B762" s="6"/>
+      <c r="B762" s="7"/>
     </row>
     <row r="763">
-      <c r="B763" s="6"/>
+      <c r="B763" s="7"/>
     </row>
     <row r="764">
-      <c r="B764" s="6"/>
+      <c r="B764" s="7"/>
     </row>
     <row r="765">
-      <c r="B765" s="6"/>
+      <c r="B765" s="7"/>
     </row>
     <row r="766">
-      <c r="B766" s="6"/>
+      <c r="B766" s="7"/>
     </row>
     <row r="767">
-      <c r="B767" s="6"/>
+      <c r="B767" s="7"/>
     </row>
     <row r="768">
-      <c r="B768" s="6"/>
+      <c r="B768" s="7"/>
     </row>
     <row r="769">
-      <c r="B769" s="6"/>
+      <c r="B769" s="7"/>
     </row>
     <row r="770">
-      <c r="B770" s="6"/>
+      <c r="B770" s="7"/>
     </row>
     <row r="771">
-      <c r="B771" s="6"/>
+      <c r="B771" s="7"/>
     </row>
     <row r="772">
-      <c r="B772" s="6"/>
+      <c r="B772" s="7"/>
     </row>
     <row r="773">
-      <c r="B773" s="6"/>
+      <c r="B773" s="7"/>
     </row>
     <row r="774">
-      <c r="B774" s="6"/>
+      <c r="B774" s="7"/>
     </row>
     <row r="775">
-      <c r="B775" s="6"/>
+      <c r="B775" s="7"/>
     </row>
     <row r="776">
-      <c r="B776" s="6"/>
+      <c r="B776" s="7"/>
     </row>
     <row r="777">
-      <c r="B777" s="6"/>
+      <c r="B777" s="7"/>
     </row>
     <row r="778">
-      <c r="B778" s="6"/>
+      <c r="B778" s="7"/>
     </row>
     <row r="779">
-      <c r="B779" s="6"/>
+      <c r="B779" s="7"/>
     </row>
     <row r="780">
-      <c r="B780" s="6"/>
+      <c r="B780" s="7"/>
     </row>
     <row r="781">
-      <c r="B781" s="6"/>
+      <c r="B781" s="7"/>
     </row>
     <row r="782">
-      <c r="B782" s="6"/>
+      <c r="B782" s="7"/>
     </row>
     <row r="783">
-      <c r="B783" s="6"/>
+      <c r="B783" s="7"/>
     </row>
     <row r="784">
-      <c r="B784" s="6"/>
+      <c r="B784" s="7"/>
     </row>
     <row r="785">
-      <c r="B785" s="6"/>
+      <c r="B785" s="7"/>
     </row>
     <row r="786">
-      <c r="B786" s="6"/>
+      <c r="B786" s="7"/>
     </row>
     <row r="787">
-      <c r="B787" s="6"/>
+      <c r="B787" s="7"/>
     </row>
     <row r="788">
-      <c r="B788" s="6"/>
+      <c r="B788" s="7"/>
     </row>
     <row r="789">
-      <c r="B789" s="6"/>
+      <c r="B789" s="7"/>
     </row>
     <row r="790">
-      <c r="B790" s="6"/>
+      <c r="B790" s="7"/>
     </row>
     <row r="791">
-      <c r="B791" s="6"/>
+      <c r="B791" s="7"/>
     </row>
     <row r="792">
-      <c r="B792" s="6"/>
+      <c r="B792" s="7"/>
     </row>
     <row r="793">
-      <c r="B793" s="6"/>
+      <c r="B793" s="7"/>
     </row>
     <row r="794">
-      <c r="B794" s="6"/>
+      <c r="B794" s="7"/>
     </row>
     <row r="795">
-      <c r="B795" s="6"/>
+      <c r="B795" s="7"/>
     </row>
     <row r="796">
-      <c r="B796" s="6"/>
+      <c r="B796" s="7"/>
     </row>
     <row r="797">
-      <c r="B797" s="6"/>
+      <c r="B797" s="7"/>
     </row>
     <row r="798">
-      <c r="B798" s="6"/>
+      <c r="B798" s="7"/>
     </row>
     <row r="799">
-      <c r="B799" s="6"/>
+      <c r="B799" s="7"/>
     </row>
     <row r="800">
-      <c r="B800" s="6"/>
+      <c r="B800" s="7"/>
     </row>
     <row r="801">
-      <c r="B801" s="6"/>
+      <c r="B801" s="7"/>
     </row>
     <row r="802">
-      <c r="B802" s="6"/>
+      <c r="B802" s="7"/>
     </row>
     <row r="803">
-      <c r="B803" s="6"/>
+      <c r="B803" s="7"/>
     </row>
     <row r="804">
-      <c r="B804" s="6"/>
+      <c r="B804" s="7"/>
     </row>
     <row r="805">
-      <c r="B805" s="6"/>
+      <c r="B805" s="7"/>
     </row>
     <row r="806">
-      <c r="B806" s="6"/>
+      <c r="B806" s="7"/>
     </row>
     <row r="807">
-      <c r="B807" s="6"/>
+      <c r="B807" s="7"/>
     </row>
     <row r="808">
-      <c r="B808" s="6"/>
+      <c r="B808" s="7"/>
     </row>
     <row r="809">
-      <c r="B809" s="6"/>
+      <c r="B809" s="7"/>
     </row>
     <row r="810">
-      <c r="B810" s="6"/>
+      <c r="B810" s="7"/>
     </row>
     <row r="811">
-      <c r="B811" s="6"/>
+      <c r="B811" s="7"/>
     </row>
     <row r="812">
-      <c r="B812" s="6"/>
+      <c r="B812" s="7"/>
     </row>
     <row r="813">
-      <c r="B813" s="6"/>
+      <c r="B813" s="7"/>
     </row>
     <row r="814">
-      <c r="B814" s="6"/>
+      <c r="B814" s="7"/>
     </row>
     <row r="815">
-      <c r="B815" s="6"/>
+      <c r="B815" s="7"/>
     </row>
     <row r="816">
-      <c r="B816" s="6"/>
+      <c r="B816" s="7"/>
     </row>
     <row r="817">
-      <c r="B817" s="6"/>
+      <c r="B817" s="7"/>
     </row>
     <row r="818">
-      <c r="B818" s="6"/>
+      <c r="B818" s="7"/>
     </row>
     <row r="819">
-      <c r="B819" s="6"/>
+      <c r="B819" s="7"/>
     </row>
     <row r="820">
-      <c r="B820" s="6"/>
+      <c r="B820" s="7"/>
     </row>
     <row r="821">
-      <c r="B821" s="6"/>
+      <c r="B821" s="7"/>
     </row>
     <row r="822">
-      <c r="B822" s="6"/>
+      <c r="B822" s="7"/>
     </row>
     <row r="823">
-      <c r="B823" s="6"/>
+      <c r="B823" s="7"/>
     </row>
     <row r="824">
-      <c r="B824" s="6"/>
+      <c r="B824" s="7"/>
     </row>
     <row r="825">
-      <c r="B825" s="6"/>
+      <c r="B825" s="7"/>
     </row>
     <row r="826">
-      <c r="B826" s="6"/>
+      <c r="B826" s="7"/>
     </row>
     <row r="827">
-      <c r="B827" s="6"/>
+      <c r="B827" s="7"/>
     </row>
     <row r="828">
-      <c r="B828" s="6"/>
+      <c r="B828" s="7"/>
     </row>
     <row r="829">
-      <c r="B829" s="6"/>
+      <c r="B829" s="7"/>
     </row>
     <row r="830">
-      <c r="B830" s="6"/>
+      <c r="B830" s="7"/>
     </row>
     <row r="831">
-      <c r="B831" s="6"/>
+      <c r="B831" s="7"/>
     </row>
     <row r="832">
-      <c r="B832" s="6"/>
+      <c r="B832" s="7"/>
     </row>
     <row r="833">
-      <c r="B833" s="6"/>
+      <c r="B833" s="7"/>
     </row>
     <row r="834">
-      <c r="B834" s="6"/>
+      <c r="B834" s="7"/>
     </row>
     <row r="835">
-      <c r="B835" s="6"/>
+      <c r="B835" s="7"/>
     </row>
     <row r="836">
-      <c r="B836" s="6"/>
+      <c r="B836" s="7"/>
     </row>
     <row r="837">
-      <c r="B837" s="6"/>
+      <c r="B837" s="7"/>
     </row>
     <row r="838">
-      <c r="B838" s="6"/>
+      <c r="B838" s="7"/>
     </row>
     <row r="839">
-      <c r="B839" s="6"/>
+      <c r="B839" s="7"/>
     </row>
     <row r="840">
-      <c r="B840" s="6"/>
+      <c r="B840" s="7"/>
     </row>
     <row r="841">
-      <c r="B841" s="6"/>
+      <c r="B841" s="7"/>
     </row>
     <row r="842">
-      <c r="B842" s="6"/>
+      <c r="B842" s="7"/>
     </row>
     <row r="843">
-      <c r="B843" s="6"/>
+      <c r="B843" s="7"/>
     </row>
     <row r="844">
-      <c r="B844" s="6"/>
+      <c r="B844" s="7"/>
     </row>
     <row r="845">
-      <c r="B845" s="6"/>
+      <c r="B845" s="7"/>
     </row>
     <row r="846">
-      <c r="B846" s="6"/>
+      <c r="B846" s="7"/>
     </row>
     <row r="847">
-      <c r="B847" s="6"/>
+      <c r="B847" s="7"/>
     </row>
     <row r="848">
-      <c r="B848" s="6"/>
+      <c r="B848" s="7"/>
     </row>
     <row r="849">
-      <c r="B849" s="6"/>
+      <c r="B849" s="7"/>
     </row>
     <row r="850">
-      <c r="B850" s="6"/>
+      <c r="B850" s="7"/>
     </row>
     <row r="851">
-      <c r="B851" s="6"/>
+      <c r="B851" s="7"/>
     </row>
     <row r="852">
-      <c r="B852" s="6"/>
+      <c r="B852" s="7"/>
     </row>
     <row r="853">
-      <c r="B853" s="6"/>
+      <c r="B853" s="7"/>
     </row>
     <row r="854">
-      <c r="B854" s="6"/>
+      <c r="B854" s="7"/>
     </row>
     <row r="855">
-      <c r="B855" s="6"/>
+      <c r="B855" s="7"/>
     </row>
     <row r="856">
-      <c r="B856" s="6"/>
+      <c r="B856" s="7"/>
     </row>
     <row r="857">
-      <c r="B857" s="6"/>
+      <c r="B857" s="7"/>
     </row>
     <row r="858">
-      <c r="B858" s="6"/>
+      <c r="B858" s="7"/>
     </row>
     <row r="859">
-      <c r="B859" s="6"/>
+      <c r="B859" s="7"/>
     </row>
     <row r="860">
-      <c r="B860" s="6"/>
+      <c r="B860" s="7"/>
     </row>
     <row r="861">
-      <c r="B861" s="6"/>
+      <c r="B861" s="7"/>
     </row>
     <row r="862">
-      <c r="B862" s="6"/>
+      <c r="B862" s="7"/>
     </row>
     <row r="863">
-      <c r="B863" s="6"/>
+      <c r="B863" s="7"/>
     </row>
     <row r="864">
-      <c r="B864" s="6"/>
+      <c r="B864" s="7"/>
     </row>
     <row r="865">
-      <c r="B865" s="6"/>
+      <c r="B865" s="7"/>
     </row>
     <row r="866">
-      <c r="B866" s="6"/>
+      <c r="B866" s="7"/>
     </row>
     <row r="867">
-      <c r="B867" s="6"/>
+      <c r="B867" s="7"/>
     </row>
     <row r="868">
-      <c r="B868" s="6"/>
+      <c r="B868" s="7"/>
     </row>
     <row r="869">
-      <c r="B869" s="6"/>
+      <c r="B869" s="7"/>
     </row>
     <row r="870">
-      <c r="B870" s="6"/>
+      <c r="B870" s="7"/>
     </row>
     <row r="871">
-      <c r="B871" s="6"/>
+      <c r="B871" s="7"/>
     </row>
     <row r="872">
-      <c r="B872" s="6"/>
+      <c r="B872" s="7"/>
     </row>
     <row r="873">
-      <c r="B873" s="6"/>
+      <c r="B873" s="7"/>
     </row>
     <row r="874">
-      <c r="B874" s="6"/>
+      <c r="B874" s="7"/>
     </row>
     <row r="875">
-      <c r="B875" s="6"/>
+      <c r="B875" s="7"/>
     </row>
     <row r="876">
-      <c r="B876" s="6"/>
+      <c r="B876" s="7"/>
     </row>
     <row r="877">
-      <c r="B877" s="6"/>
+      <c r="B877" s="7"/>
     </row>
     <row r="878">
-      <c r="B878" s="6"/>
+      <c r="B878" s="7"/>
     </row>
     <row r="879">
-      <c r="B879" s="6"/>
+      <c r="B879" s="7"/>
     </row>
     <row r="880">
-      <c r="B880" s="6"/>
+      <c r="B880" s="7"/>
     </row>
     <row r="881">
-      <c r="B881" s="6"/>
+      <c r="B881" s="7"/>
     </row>
     <row r="882">
-      <c r="B882" s="6"/>
+      <c r="B882" s="7"/>
     </row>
     <row r="883">
-      <c r="B883" s="6"/>
+      <c r="B883" s="7"/>
     </row>
     <row r="884">
-      <c r="B884" s="6"/>
+      <c r="B884" s="7"/>
     </row>
     <row r="885">
-      <c r="B885" s="6"/>
+      <c r="B885" s="7"/>
     </row>
     <row r="886">
-      <c r="B886" s="6"/>
+      <c r="B886" s="7"/>
     </row>
     <row r="887">
-      <c r="B887" s="6"/>
+      <c r="B887" s="7"/>
     </row>
     <row r="888">
-      <c r="B888" s="6"/>
+      <c r="B888" s="7"/>
     </row>
     <row r="889">
-      <c r="B889" s="6"/>
+      <c r="B889" s="7"/>
     </row>
     <row r="890">
-      <c r="B890" s="6"/>
+      <c r="B890" s="7"/>
     </row>
     <row r="891">
-      <c r="B891" s="6"/>
+      <c r="B891" s="7"/>
     </row>
     <row r="892">
-      <c r="B892" s="6"/>
+      <c r="B892" s="7"/>
     </row>
     <row r="893">
-      <c r="B893" s="6"/>
+      <c r="B893" s="7"/>
     </row>
     <row r="894">
-      <c r="B894" s="6"/>
+      <c r="B894" s="7"/>
     </row>
     <row r="895">
-      <c r="B895" s="6"/>
+      <c r="B895" s="7"/>
     </row>
     <row r="896">
-      <c r="B896" s="6"/>
+      <c r="B896" s="7"/>
     </row>
     <row r="897">
-      <c r="B897" s="6"/>
+      <c r="B897" s="7"/>
     </row>
     <row r="898">
-      <c r="B898" s="6"/>
+      <c r="B898" s="7"/>
     </row>
     <row r="899">
-      <c r="B899" s="6"/>
+      <c r="B899" s="7"/>
     </row>
     <row r="900">
-      <c r="B900" s="6"/>
+      <c r="B900" s="7"/>
     </row>
     <row r="901">
-      <c r="B901" s="6"/>
+      <c r="B901" s="7"/>
     </row>
     <row r="902">
-      <c r="B902" s="6"/>
+      <c r="B902" s="7"/>
     </row>
     <row r="903">
-      <c r="B903" s="6"/>
+      <c r="B903" s="7"/>
     </row>
     <row r="904">
-      <c r="B904" s="6"/>
+      <c r="B904" s="7"/>
     </row>
     <row r="905">
-      <c r="B905" s="6"/>
+      <c r="B905" s="7"/>
     </row>
     <row r="906">
-      <c r="B906" s="6"/>
+      <c r="B906" s="7"/>
     </row>
     <row r="907">
-      <c r="B907" s="6"/>
+      <c r="B907" s="7"/>
     </row>
     <row r="908">
-      <c r="B908" s="6"/>
+      <c r="B908" s="7"/>
     </row>
     <row r="909">
-      <c r="B909" s="6"/>
+      <c r="B909" s="7"/>
     </row>
     <row r="910">
-      <c r="B910" s="6"/>
+      <c r="B910" s="7"/>
     </row>
     <row r="911">
-      <c r="B911" s="6"/>
+      <c r="B911" s="7"/>
     </row>
     <row r="912">
-      <c r="B912" s="6"/>
+      <c r="B912" s="7"/>
     </row>
     <row r="913">
-      <c r="B913" s="6"/>
+      <c r="B913" s="7"/>
     </row>
     <row r="914">
-      <c r="B914" s="6"/>
+      <c r="B914" s="7"/>
     </row>
     <row r="915">
-      <c r="B915" s="6"/>
+      <c r="B915" s="7"/>
     </row>
     <row r="916">
-      <c r="B916" s="6"/>
+      <c r="B916" s="7"/>
     </row>
     <row r="917">
-      <c r="B917" s="6"/>
+      <c r="B917" s="7"/>
     </row>
     <row r="918">
-      <c r="B918" s="6"/>
+      <c r="B918" s="7"/>
     </row>
     <row r="919">
-      <c r="B919" s="6"/>
+      <c r="B919" s="7"/>
     </row>
     <row r="920">
-      <c r="B920" s="6"/>
+      <c r="B920" s="7"/>
     </row>
     <row r="921">
-      <c r="B921" s="6"/>
+      <c r="B921" s="7"/>
     </row>
     <row r="922">
-      <c r="B922" s="6"/>
+      <c r="B922" s="7"/>
     </row>
     <row r="923">
-      <c r="B923" s="6"/>
+      <c r="B923" s="7"/>
     </row>
     <row r="924">
-      <c r="B924" s="6"/>
+      <c r="B924" s="7"/>
     </row>
     <row r="925">
-      <c r="B925" s="6"/>
+      <c r="B925" s="7"/>
     </row>
     <row r="926">
-      <c r="B926" s="6"/>
+      <c r="B926" s="7"/>
     </row>
     <row r="927">
-      <c r="B927" s="6"/>
+      <c r="B927" s="7"/>
     </row>
     <row r="928">
-      <c r="B928" s="6"/>
+      <c r="B928" s="7"/>
     </row>
     <row r="929">
-      <c r="B929" s="6"/>
+      <c r="B929" s="7"/>
     </row>
     <row r="930">
-      <c r="B930" s="6"/>
+      <c r="B930" s="7"/>
     </row>
     <row r="931">
-      <c r="B931" s="6"/>
+      <c r="B931" s="7"/>
     </row>
     <row r="932">
-      <c r="B932" s="6"/>
+      <c r="B932" s="7"/>
     </row>
     <row r="933">
-      <c r="B933" s="6"/>
+      <c r="B933" s="7"/>
     </row>
     <row r="934">
-      <c r="B934" s="6"/>
+      <c r="B934" s="7"/>
     </row>
     <row r="935">
-      <c r="B935" s="6"/>
+      <c r="B935" s="7"/>
     </row>
     <row r="936">
-      <c r="B936" s="6"/>
+      <c r="B936" s="7"/>
     </row>
     <row r="937">
-      <c r="B937" s="6"/>
+      <c r="B937" s="7"/>
     </row>
     <row r="938">
-      <c r="B938" s="6"/>
+      <c r="B938" s="7"/>
     </row>
     <row r="939">
-      <c r="B939" s="6"/>
+      <c r="B939" s="7"/>
     </row>
     <row r="940">
-      <c r="B940" s="6"/>
+      <c r="B940" s="7"/>
     </row>
     <row r="941">
-      <c r="B941" s="6"/>
+      <c r="B941" s="7"/>
     </row>
     <row r="942">
-      <c r="B942" s="6"/>
+      <c r="B942" s="7"/>
     </row>
     <row r="943">
-      <c r="B943" s="6"/>
+      <c r="B943" s="7"/>
     </row>
     <row r="944">
-      <c r="B944" s="6"/>
+      <c r="B944" s="7"/>
     </row>
     <row r="945">
-      <c r="B945" s="6"/>
+      <c r="B945" s="7"/>
     </row>
     <row r="946">
-      <c r="B946" s="6"/>
+      <c r="B946" s="7"/>
     </row>
     <row r="947">
-      <c r="B947" s="6"/>
+      <c r="B947" s="7"/>
     </row>
     <row r="948">
-      <c r="B948" s="6"/>
+      <c r="B948" s="7"/>
     </row>
     <row r="949">
-      <c r="B949" s="6"/>
+      <c r="B949" s="7"/>
     </row>
     <row r="950">
-      <c r="B950" s="6"/>
+      <c r="B950" s="7"/>
     </row>
     <row r="951">
-      <c r="B951" s="6"/>
+      <c r="B951" s="7"/>
     </row>
     <row r="952">
-      <c r="B952" s="6"/>
+      <c r="B952" s="7"/>
     </row>
     <row r="953">
-      <c r="B953" s="6"/>
+      <c r="B953" s="7"/>
     </row>
     <row r="954">
-      <c r="B954" s="6"/>
+      <c r="B954" s="7"/>
     </row>
     <row r="955">
-      <c r="B955" s="6"/>
+      <c r="B955" s="7"/>
     </row>
     <row r="956">
-      <c r="B956" s="6"/>
+      <c r="B956" s="7"/>
     </row>
     <row r="957">
-      <c r="B957" s="6"/>
+      <c r="B957" s="7"/>
     </row>
     <row r="958">
-      <c r="B958" s="6"/>
+      <c r="B958" s="7"/>
     </row>
     <row r="959">
-      <c r="B959" s="6"/>
+      <c r="B959" s="7"/>
     </row>
     <row r="960">
-      <c r="B960" s="6"/>
+      <c r="B960" s="7"/>
     </row>
     <row r="961">
-      <c r="B961" s="6"/>
+      <c r="B961" s="7"/>
     </row>
     <row r="962">
-      <c r="B962" s="6"/>
+      <c r="B962" s="7"/>
     </row>
     <row r="963">
-      <c r="B963" s="6"/>
+      <c r="B963" s="7"/>
     </row>
     <row r="964">
-      <c r="B964" s="6"/>
+      <c r="B964" s="7"/>
     </row>
     <row r="965">
-      <c r="B965" s="6"/>
+      <c r="B965" s="7"/>
     </row>
     <row r="966">
-      <c r="B966" s="6"/>
+      <c r="B966" s="7"/>
     </row>
     <row r="967">
-      <c r="B967" s="6"/>
+      <c r="B967" s="7"/>
     </row>
     <row r="968">
-      <c r="B968" s="6"/>
+      <c r="B968" s="7"/>
     </row>
     <row r="969">
-      <c r="B969" s="6"/>
+      <c r="B969" s="7"/>
     </row>
     <row r="970">
-      <c r="B970" s="6"/>
+      <c r="B970" s="7"/>
     </row>
     <row r="971">
-      <c r="B971" s="6"/>
+      <c r="B971" s="7"/>
     </row>
     <row r="972">
-      <c r="B972" s="6"/>
+      <c r="B972" s="7"/>
     </row>
     <row r="973">
-      <c r="B973" s="6"/>
+      <c r="B973" s="7"/>
     </row>
     <row r="974">
-      <c r="B974" s="6"/>
+      <c r="B974" s="7"/>
     </row>
     <row r="975">
-      <c r="B975" s="6"/>
+      <c r="B975" s="7"/>
     </row>
     <row r="976">
-      <c r="B976" s="6"/>
+      <c r="B976" s="7"/>
     </row>
     <row r="977">
-      <c r="B977" s="6"/>
+      <c r="B977" s="7"/>
     </row>
     <row r="978">
-      <c r="B978" s="6"/>
+      <c r="B978" s="7"/>
     </row>
     <row r="979">
-      <c r="B979" s="6"/>
+      <c r="B979" s="7"/>
     </row>
     <row r="980">
-      <c r="B980" s="6"/>
+      <c r="B980" s="7"/>
     </row>
     <row r="981">
-      <c r="B981" s="6"/>
+      <c r="B981" s="7"/>
     </row>
     <row r="982">
-      <c r="B982" s="6"/>
+      <c r="B982" s="7"/>
     </row>
     <row r="983">
-      <c r="B983" s="6"/>
+      <c r="B983" s="7"/>
     </row>
     <row r="984">
-      <c r="B984" s="6"/>
+      <c r="B984" s="7"/>
     </row>
     <row r="985">
-      <c r="B985" s="6"/>
+      <c r="B985" s="7"/>
     </row>
     <row r="986">
-      <c r="B986" s="6"/>
+      <c r="B986" s="7"/>
     </row>
     <row r="987">
-      <c r="B987" s="6"/>
+      <c r="B987" s="7"/>
     </row>
     <row r="988">
-      <c r="B988" s="6"/>
+      <c r="B988" s="7"/>
     </row>
     <row r="989">
-      <c r="B989" s="6"/>
+      <c r="B989" s="7"/>
     </row>
     <row r="990">
-      <c r="B990" s="6"/>
+      <c r="B990" s="7"/>
     </row>
     <row r="991">
-      <c r="B991" s="6"/>
+      <c r="B991" s="7"/>
     </row>
     <row r="992">
-      <c r="B992" s="6"/>
+      <c r="B992" s="7"/>
     </row>
     <row r="993">
-      <c r="B993" s="6"/>
+      <c r="B993" s="7"/>
     </row>
     <row r="994">
-      <c r="B994" s="6"/>
+      <c r="B994" s="7"/>
     </row>
     <row r="995">
-      <c r="B995" s="6"/>
+      <c r="B995" s="7"/>
     </row>
     <row r="996">
-      <c r="B996" s="6"/>
+      <c r="B996" s="7"/>
     </row>
     <row r="997">
-      <c r="B997" s="6"/>
+      <c r="B997" s="7"/>
     </row>
     <row r="998">
-      <c r="B998" s="6"/>
+      <c r="B998" s="7"/>
     </row>
     <row r="999">
-      <c r="B999" s="6"/>
+      <c r="B999" s="7"/>
     </row>
     <row r="1000">
-      <c r="B1000" s="6"/>
+      <c r="B1000" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink r:id="rId2" ref="B5"/>
+    <hyperlink r:id="rId3" ref="B9"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>